<commit_message>
try running with expressJS
</commit_message>
<xml_diff>
--- a/cypress/downloads/out1.xlsx
+++ b/cypress/downloads/out1.xlsx
@@ -489,14 +489,12 @@
       </c>
       <c r="H3" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	 2011-2020 yılları arasında biyoçeşitliliğin korunmasına ilişkin eğitimde biyoçeşitliliğin daha iyi anlaşılmasını sağlamak için eğitimin öğrencilerden başlanarak yapılması gerektiği vurgulanmıştır. Bu nedenle, fen öğretmenlerinin biyoçeşitlilik ile ilgili konularda bilgi sahibi olmaları için biyoçeşitlilik eğitiminin öğretmenlik eğitimine entegrasyonunun sağlanması gerekmektedir. Bu araştırmanın amacı, ortaokul fen öğretmenlerinin biyoçeşitlilik hakkındaki görüşlerini ortaya koymaktır. Araştırmada nitel araştırma yöntemlerinden biri olarak anılan durum çalışması benimsenmiştir. Araştırmanın çalışma grubunu, Zambiya'nın Lusaka ilinde kasıtlı olarak seçilen 8 ortaokulda görev yapmakta olan 30 fen öğretmeni oluşturmaktadır. Araştırmanın verileri, 30 fen öğretmeni ile kişisel görüşmeler yapılarak yarı yapılandırılmış görüşme formları ile toplanmıştır. Araştırma sonuçlarına göre fen öğretmenlerinin biyoçeşitlilik kavramını çevreleyen bilimsel temeller hakkında derinlemesine bir anlayışa sahip olmadığı sonucuna varılmıştır. Fen öğretmenlerinin biyoçeşitliliğin azalmasına yol açan faktörler hakkında bilgileri iyi düzeydedir. Ayrıca biyoçeşitliliğin değeri konusunda da iyi bir anlayışa sahiptirler. Fen öğretmenlerinin biyolojik çeşitliliğin korunmasını sağlamada kendilerinden ne beklendiğini çok iyi anladıkları sonucuna varılmıştır. Araştırmanın bir diğer sonuçları, biyoçeşitlilik eğitiminin etkin ve geliştirilmiş duyarlılaştırılmasına yapılan vurgunun biyoçeşitlilik eğitiminin pazarlanmasına yardımcı olacağıdır. Sürdürülebilir topluluk biyoçeşitlilik bilincini oluşturmaya ve geliştirmeye yardımcı olacaktır. Biyoçeşitlilik duyarlılık programlarının oluşturulması gerekmektedir. Biyoçeşitliliğin korunmasını sağlayan bir politikanın oluşturulması, biyoçeşitliliğin korunması yasasının Zambiya'da gerektiği gibi uygulanmasını sağlayacaktır. Biyoçeşitlilik eğitimi hakkında birinci el bilgi taşıyıcıları olarak fen öğretmenlerine biyoçeşitlilik eğitimi verilmesi, biyoçeşitliliğin korunmasını sağlamanın merkezinde yer alan öğretmenlerin biyoçeşitliliğin korunması konusunda iyi donanımlı olmalarını sağlayacaktır.  Sonuç olarak, sürdürülebilir enerji kaynaklarının kullanımı sonucunda ormanların zarar görmesi engellenmiş ve  biyoçeşitlilik korunmuş olacaktır.
-Anahtar Kelimeler: Biyolojik Çeşitlilik, Çevre Eğitimi, Fen Öğretmenleri
+	 Günümüzde çevre kirliliği ile birlikte biyoçeşitlilik kaybı da artmaktadır. Biyoçeşitlilik kaybını anlamada biyoçeşitlilik okuryazarlığı önem kazanmaktadır. Biyoçeşitlilik okuryazarlığında, edinilen bilginin anlamlandırılmasında eleştirel düşünme önemli bir yere sahip olan faktörlerden biridir. Bu araştırmada, fen bilgisi öğretmen adaylarının eleştirel düşünme becerileri ve biyoçeşitlilik okuryazarlığı arasındaki ilişkiyi inceleme amaçlanmıştır. Araştırmada, Ege Bölgesinde bulunan 5 farklı üniversitede öğrenim gören 224 fen bilgisi öğretmen adayı katılmıştır. Araştırmada karşılaştırmalı nedensel ve ilişkisel araştırma yöntemleri birlikte işe koşulmuştur. Verileri toplamada Yoldaş [30] tarafından geliştirilen ve Cronbach Alpha güvenirliği 0,87 olan Eleştirel Düşünme Becerileri Ölçeği (EDBÖ) ve Gürbüz ve ark. [109] tarafından geliştirilen ve Cronbach Alpha güvenirliği 0,85 olan Biyoçeşitlilik Okuryazarlığı Ölçeği (BOÖ) kullanılmış olup, verilerin analizi SPSS 15. programında yapılmıştır. EDBÖ, eleştirel düşünmede hassasiyet, eleştirel düşünmede bilinç, eleştirel düşünmede empati, eleştirel düşünmede kabullenme, eleştirel düşünmede varsayımlar, eleştirel düşünmede sağduyu ve medyaya yönelik eleştirel düşünme becerileri olmak üzere 7 faktörden oluşmaktadır. BOÖ, biyoçeşitlilik tehdit unsurları, biyoçeşitlilik kavramı ve biyoçeşitlilik önemi olmak üzere 3 faktörden oluşmaktadır. Araştırmada verilerin analizinde bağımsız örneklemli t-testi, ANOVA tek yönlü faktör analizi, korelasyon analizi, basit doğrusal regresyon analizi ve ölçeklerin faktörleri arasındaki ilişkiyi araştırmak için kanonik korelasyon analizi yapılmıştır. Çalışma sonucunda, öğretmen adaylarının cinsiyet değişkenine bağlı eleştirel düşünme becerilerinde anlamlı bir farklılığın olduğu görülmüştür. Ayrıca öğretmen adaylarının eleştirel düşünme becerileri ve biyoçeşitlilik okuryazarlığı arasında pozitif yönde düşük ve anlamlı bir ilişkinin olduğu tespit edilmiştir. Öğretmen adaylarının eleştirel düşünme becerileri, biyoçeşitlilik okuryazarlığını anlamlı bir şekilde yordadığı ve varyansın %5,1'ini açıkladığı yapılan basit doğrusal regresyon analizi sonucunda tespit edilmiştir. EDBÖ "Eleştirel Düşünmede Empati" faktörü ile BOÖ "Biyoçeşitlilik Kavramı" faktörü arasında anlamlı bir ilişkinin olduğu yapılan kanonik korelasyon analizi sonucunda tespit edilmiştir. Fen bilgisi öğretmen adaylarının eleştirel düşünme becerilerinde, yaş ve sınıf değişkenleri açısından anlamlı bir farklılığın olmadığı gözlenmiştir. Öğretmen adaylarının biyoçeşitlilik okuryazarlığında, cinsiyet, yaş ve sınıf değişkenleri açısından anlamlı bir farklılığın olmadığı tespit edilmiştir.
 	 </v>
       </c>
       <c r="I3" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	  It has been emphasized that education should be started from students in order to provide a better understanding of biodiversity in education on the protection of biodiversity between the years 2011-2020. For this reason, it is necessary to integrate biodiversity education into teacher education so that science teachers have knowledge about biodiversity-related issues. The aim of this research is to reveal the views of secondary school science teachers about biodiversity. The case study, which is known as one of the qualitative research methods, was adopted in the research. The study group of the research consists of 30 science teachers working in 8 deliberately selected secondary schools in Lusaka, Zambia. The data of the study were collected through semi-structured interview form by making personal interviews with 30 science teachers. According to the results of the research, it was concluded that science teachers do not have an in-depth understanding of the scientific foundations surrounding the concept of biodiversity. Science teachers have a good level of knowledge about the factors that lead to the reduction of biodiversity. They also have a good understanding of the value of biodiversity. It has been concluded that science teachers understand very well what is expected of them in ensuring the protection of biological diversity. Another conclusion of the research is that the emphasis on effective and improved sensitization of biodiversity education will help in the marketing of biodiversity education. Sustainable community will help build and improve biodiversity awareness. Biodiversity awareness programs need to be established. Establishing a policy that ensures biodiversity conservation will ensure that biodiversity conservation law is properly implemented in Zambia. Providing biodiversity education to science teachers as first-hand information carriers about biodiversity education will ensure that teachers, who are at the center of ensuring biodiversity conservation, are well-equipped for biodiversity conservation. As a result, damage to forests will be prevented and biodiversity will be protected as a result of the use of sustainable energy resources.
-Keywords: Biodiversity, Biodiversity, Environmental Education, Science Teachers</v>
+	  Today, along with environmental pollution, biodiversity loss is increasing. Biodiversity literacy is critical to understanding biodiversity loss. In biodiversity literacy, critical thinking is one of the factors that has an important place in making sense of the acquired knowledge. This study, aimed to examine the relationship between the critical thinking skills of pre-service science teachers and biodiversity literacy. 224 pre-service science teachers studying at 5 different universities in the Aegean region participated in the study. In the study, comparative causal and relational research methods were employed together. In collecting the data, Yoldaş's Critical Thinking Skills Scale (CTSS) [30] (with a Cronbach Alpha reliability of 0.87) and the Biodiversity Literacy Scale (BLS), developed by Gürbüz et al, [109] (whit a Cronbach Alpha reliability of 0.85), were used. Analysis of the data was performed using the SPSS 15. The CTSS consists of 7 factors: sensitivity in critical thinking, awareness in critical thinking, empathy in critical thinking, acceptance in critical thinking, assumptions in critical thinking, common sense in critical thinking, and thinking critically about the media. The BLS consists of three factors: biodiversity threats, the concept of biodiversity, and the importance of biodiversity. In the analysis of the data, an independent sample t-test, ANOVA one-way factor analysis, correlation analysis, simple linear regression analysis, and canonical correlation analysis were used to investigate the relationship between the factors of the scales. As a result of the study, it was seen that there was a significant difference in the critical thinking skills of the teacher candidates depending on the gender variable. In addition, it was determined that there is a low and significant positive relationship between pre-service teachers' critical thinking skills and biodiversity literacy. The critical thinking skills of pre-service teachers were determined as a result of simple linear regression analysis that significantly predicted biodiversity literacy and explained 5.1% of the variance. As a result of the canonical correlation analysis, it was determined that there was a significant relationship between the "Empathy in Critical Thinking" factor and the NCD "Concept of Biodiversity" factor. No significant difference in the critical thinking skills of science teacher candidates in terms of age and class variables was observed. It was also determined that there is no significant difference in the biodiversity literacy of teacher candidates in terms of gender, age, and class variables.</v>
       </c>
     </row>
     <row r="4" xml:space="preserve">
@@ -523,12 +521,14 @@
       </c>
       <c r="H4" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	 Günümüzde çevre kirliliği ile birlikte biyoçeşitlilik kaybı da artmaktadır. Biyoçeşitlilik kaybını anlamada biyoçeşitlilik okuryazarlığı önem kazanmaktadır. Biyoçeşitlilik okuryazarlığında, edinilen bilginin anlamlandırılmasında eleştirel düşünme önemli bir yere sahip olan faktörlerden biridir. Bu araştırmada, fen bilgisi öğretmen adaylarının eleştirel düşünme becerileri ve biyoçeşitlilik okuryazarlığı arasındaki ilişkiyi inceleme amaçlanmıştır. Araştırmada, Ege Bölgesinde bulunan 5 farklı üniversitede öğrenim gören 224 fen bilgisi öğretmen adayı katılmıştır. Araştırmada karşılaştırmalı nedensel ve ilişkisel araştırma yöntemleri birlikte işe koşulmuştur. Verileri toplamada Yoldaş [30] tarafından geliştirilen ve Cronbach Alpha güvenirliği 0,87 olan Eleştirel Düşünme Becerileri Ölçeği (EDBÖ) ve Gürbüz ve ark. [109] tarafından geliştirilen ve Cronbach Alpha güvenirliği 0,85 olan Biyoçeşitlilik Okuryazarlığı Ölçeği (BOÖ) kullanılmış olup, verilerin analizi SPSS 15. programında yapılmıştır. EDBÖ, eleştirel düşünmede hassasiyet, eleştirel düşünmede bilinç, eleştirel düşünmede empati, eleştirel düşünmede kabullenme, eleştirel düşünmede varsayımlar, eleştirel düşünmede sağduyu ve medyaya yönelik eleştirel düşünme becerileri olmak üzere 7 faktörden oluşmaktadır. BOÖ, biyoçeşitlilik tehdit unsurları, biyoçeşitlilik kavramı ve biyoçeşitlilik önemi olmak üzere 3 faktörden oluşmaktadır. Araştırmada verilerin analizinde bağımsız örneklemli t-testi, ANOVA tek yönlü faktör analizi, korelasyon analizi, basit doğrusal regresyon analizi ve ölçeklerin faktörleri arasındaki ilişkiyi araştırmak için kanonik korelasyon analizi yapılmıştır. Çalışma sonucunda, öğretmen adaylarının cinsiyet değişkenine bağlı eleştirel düşünme becerilerinde anlamlı bir farklılığın olduğu görülmüştür. Ayrıca öğretmen adaylarının eleştirel düşünme becerileri ve biyoçeşitlilik okuryazarlığı arasında pozitif yönde düşük ve anlamlı bir ilişkinin olduğu tespit edilmiştir. Öğretmen adaylarının eleştirel düşünme becerileri, biyoçeşitlilik okuryazarlığını anlamlı bir şekilde yordadığı ve varyansın %5,1'ini açıkladığı yapılan basit doğrusal regresyon analizi sonucunda tespit edilmiştir. EDBÖ "Eleştirel Düşünmede Empati" faktörü ile BOÖ "Biyoçeşitlilik Kavramı" faktörü arasında anlamlı bir ilişkinin olduğu yapılan kanonik korelasyon analizi sonucunda tespit edilmiştir. Fen bilgisi öğretmen adaylarının eleştirel düşünme becerilerinde, yaş ve sınıf değişkenleri açısından anlamlı bir farklılığın olmadığı gözlenmiştir. Öğretmen adaylarının biyoçeşitlilik okuryazarlığında, cinsiyet, yaş ve sınıf değişkenleri açısından anlamlı bir farklılığın olmadığı tespit edilmiştir.
+	 Araştırmanın amacı, biyoçeşitlilik konusunda yazılı, görsel ve işitsel medya kullanımının biyoloji öğretmen adaylarının biyoçeşitlilik okuryazarlığı, akademik başarıları ve biyoçeşitlilik öğretiminde medya kullanılmasına yönelik görüşleri üzerine etkisini araştırmaktır. Araştırma verilerinin toplanmasında nicel ve nitel veri toplama yöntemlerinin bir arada kullanıldığı karma yöntem uygulanmıştır. Araştırmanın nicel kısmında, deneysel modellerden "tek grup öntest-sontest desen", nitel kısmında açık uçlu anket soruları kullanılmıştır. Araştırma 2014-2015 eğitim-öğretim yılında Gazi Üniversitesi, Biyoloji Eğitimi Ana Bilim Dalı 3. sınıfında okuyan 21 öğrenci ile yapılmıştır. Araştırmada veriler biyoçeşitlilik okuryazarlığı ölçeği, araştırmacı tarafından geliştirilen biyoçeşitlilik başarı testi ve açık uçlu anket soruları ile toplanmıştır. Araştırmada öntest olarak; biyoçeşitlilik başarı testi, biyoçeşitlilik okuryazarlığı ölçeği uygulanmıştır. Uygulamanın ardından öntestte uygulanan testler sontest olarak tekrar uygulanmış ve öğrencilerin görüşlerini almak için açık uçlu anket soruları uygulanmıştır. Verilerin analizi için SPSS 21 istatistik programı kullanılmıştır. Araştırma sonucunda, biyoloji öğretmen adaylarının biyoçeşitlilik başarı testinden aldıkları uygulama öncesi ve sonrası puanlarının arasında anlamlı bir fark olduğu görülmüştür. Biyoloji öğretmen adaylarının biyoçeşitlilik okuryazarlığı ölçeğinden aldıkları uygulama öncesi ve sonrası puanların arasında anlamlı bir fark bulunmamıştır. Araştırmada biyoçeşitlilik konusunda yazılı, görsel ve işitsel medya kullanılarak uygulanan öğretimden sonra biyoloji öğretmen adaylarından alınan öğretimde medya kullanılmasına yönelik görüşlerinin olumlu olduğu belirlenmiştir.
+Anahtar Kelimeler : Biyoçeşitlilik, Biyoçeşitlilik okuryazarlığı, Medya kullanımı, Çevre eğitimi
 	 </v>
       </c>
       <c r="I4" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	  Today, along with environmental pollution, biodiversity loss is increasing. Biodiversity literacy is critical to understanding biodiversity loss. In biodiversity literacy, critical thinking is one of the factors that has an important place in making sense of the acquired knowledge. This study, aimed to examine the relationship between the critical thinking skills of pre-service science teachers and biodiversity literacy. 224 pre-service science teachers studying at 5 different universities in the Aegean region participated in the study. In the study, comparative causal and relational research methods were employed together. In collecting the data, Yoldaş's Critical Thinking Skills Scale (CTSS) [30] (with a Cronbach Alpha reliability of 0.87) and the Biodiversity Literacy Scale (BLS), developed by Gürbüz et al, [109] (whit a Cronbach Alpha reliability of 0.85), were used. Analysis of the data was performed using the SPSS 15. The CTSS consists of 7 factors: sensitivity in critical thinking, awareness in critical thinking, empathy in critical thinking, acceptance in critical thinking, assumptions in critical thinking, common sense in critical thinking, and thinking critically about the media. The BLS consists of three factors: biodiversity threats, the concept of biodiversity, and the importance of biodiversity. In the analysis of the data, an independent sample t-test, ANOVA one-way factor analysis, correlation analysis, simple linear regression analysis, and canonical correlation analysis were used to investigate the relationship between the factors of the scales. As a result of the study, it was seen that there was a significant difference in the critical thinking skills of the teacher candidates depending on the gender variable. In addition, it was determined that there is a low and significant positive relationship between pre-service teachers' critical thinking skills and biodiversity literacy. The critical thinking skills of pre-service teachers were determined as a result of simple linear regression analysis that significantly predicted biodiversity literacy and explained 5.1% of the variance. As a result of the canonical correlation analysis, it was determined that there was a significant relationship between the "Empathy in Critical Thinking" factor and the NCD "Concept of Biodiversity" factor. No significant difference in the critical thinking skills of science teacher candidates in terms of age and class variables was observed. It was also determined that there is no significant difference in the biodiversity literacy of teacher candidates in terms of gender, age, and class variables.</v>
+	  The purpose of this study is research the effect of usage written, visual and audio media on biodiversity upon biodiversity literacy and academic achievement their opinions regarding the use of media in biodiversity teaching of pre-service biology teachers. Mixed method in which quantitative and qualitative data collecting methods are used together is applied on collecting data of research. On quantitative part of research, single group pro-test post-test puttern, on qualitative part open-ended survey questions are wed. Research was done with 21 3rd grade Gazi University, Faculty of Education, Department of Biology Education students in 2014-2015 academic year. In research, datas were collected with scale of biodiversity literacy , biodiversity success test and open-ended survey questions that were developed by researcher. In research, biodiversity success test, scale of biodiversity literacy were applied as a pre-test. After application, tests that werw applied in pre-test were applied again as a post-test and for the sake of having student's view, open-ended survey questions were applied. The data obtained from these tests were analyzed by the use of SPSS statistical software. At the end of the research, it was seen that there was a big differences between biology teacher candidates' marks that were taken before and after application. Big differences wasn't found between biology teacher candidate's mark that were taken before and after application from scale of biodiversity literacy. In research, after teaching about biodiversity subject that is wed with written, visual and audial media opinions from biology teacher candidates about media usage on teaching were determined as a positive.
+Key Words : Biodiversity, Biodiversity literacy, Usage of media, Environmental education</v>
       </c>
     </row>
     <row r="5" xml:space="preserve">
@@ -589,55 +589,12 @@
       </c>
       <c r="H6" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	 Biyoçeşitlilik sürdürülebilir ormancılık çalışmalarının en önemli unsurlarındandır.
-Ancak Türkiye'de ormancıların eğitim ve profesyonel gelişim programlarında yeterli bir
-şekilde yer almamaktadır. Her ne kadar biyoçeşitlilik eğitimini ormancılık ile
-bütünleştirme çalışmaları yapıldıysa da, bunlar istenilen seviyede olamamıştır. Orman
-mühendisliği eğitiminde biyoçeşitlilik konusunda büyük bir boşluk vardır. Bu çalışma
-biyoçeşitlilik eğitimini daha düşük zaman ve maaliyet ile yaygınlaştırılması için
-geliştirilecek çevrimiçi destek aracı ile bu boşluğu doldurmayı hedeflemektedir.
-Bu çalışmanın asıl amacı geliştirilecek web tabanlı aracın, Türkiye'deki ormancıların
-biyoçeşitlilik eğitiminin yaygınlaştırılması için geçerli bir çözüm olabilme potansiyelini
-araştırmaktır. Bu araştırma, biyoçeşitlilik eğitimi için çevrimiçi destek aracının
-tasarımını, geliştirilmesini ve değerlendirmesini kapsayan tasarım ve geliştirme
-araştırma yöntemi kullanılmıştır. Denekler amaca yönelik örneklem tekniği ile orman
-genel müdürlüğü bünyesinde çalışan orman mühendisleri arasından seçilmiştir. Geliştirilen web tabanlı aracın kalitesi talepten doğan öğrenme modeli teorik yapıya
-dayandırılarak sağlanmıştır.
-Anket soruları, görüşme oturumları ve sistem kayıtlarına bakıldığında, katılımcıların
-çalışma kapsamında tasarlanan ve geliştirilen araç hakkında olumlu görüşleri olduğu
-görüldü. Bunun yanı sıra, katılımcılar bu eğitim programı ile profesyonel hayatlarında
-kullanacakları yeni bilgiler kazandıklarını belirttiler. Katılımcıların araştırmanın teorik
-çerçevesinin tüm karakteristiklerine karşı tutumları olumlu bulundu. Ayrıca araştırmanın
-sonuçları, katılımcıların eğitim aracını uygun bulduklarını ve çevrimiçi eğitim
-programlarına karşı tutumlarının değiştiğini gösterdi.
-Anahtar Kelimeler: tasarım ve geliştirme araştırma yöntemi, talepten doğan öğrenme 
-modeli, biyoçeşitlilik eğitimi
+	 Bu araştırma, biyoloji öğretmenleri için biyoçeşitlilik konusunda rehber eğitim materyali hazırlamak amacıyla yapılmıştır. Görüşme yönteminin kullanıldığı araştırmada, Ankara İli merkez ilçelerinde görevli 37 gönüllü biyoloji öğretmeninden oluşan örneklem grubunun, hazırlanan rehber materyal hakkındaki görüşleri ve biyoçeşitlilik öğretimi konusundaki önerileri alınmıştır.Öğretmenlerin ?biyoçeşitlilikle ilgili bilgi düzeyleri? ve ?biyoçeşitlilik eğitimine ilişkin yeterlilik algıları?; cinsiyet, mesleki deneyim, görev yaptıkları okul türü, sınıfta bulunan ortalama öğrenci sayısı ve mezun oldukları fakülte değişkenlerine göre X2 (Ki-kare) testi yapılarak değerlendirilmiştir. Öğretmenlerin ?biyoçeşitlilik eğitimine ilişkin yeterlilik algısı? ile ?biyoçeşitlilikle ilgili bilgi düzeyleri? arasındaki ilişki anlamlı bulunmuştur.Bu çalışma sonucunda; biyoçeşitlilik öğretimi hakkında önerilerde bulunan 15 öğretmen uygulamalı eğitimin öneminden bahsetmiştir. Araştırmaya katılan 21 öğretmen hazırlanan rehber materyali çok beğenmiş, 17 öğretmen de materyalin bilgi düzeyini artırdığını belirtmiştir.Biyoçeşitlilik konusunda hazırlanan rehber materyal mineseckinkurumlu @gmail.com adresinden araştırmacı ile irtibata geçilerek istek yapılabilir.
 	 </v>
       </c>
       <c r="I6" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	  Biodiversity is one of the most important elements of the sustainable forestry practices.
-However, in Turkey biodiversity is not properly included in the forestry training
-curriculum and in professional training. There is a gap in the education of forest
-engineering about biodiversity. This study aims to fill this gap by developing an online
-support tool targeting dissemination of the biodiversity training with lower cost and
-time.
-The primary aim of this study is to explore the potential of web based tool as a viable
-solution to dissemination of the biodiversity training to forest engineers in Turkey. This
-research based on design and development research methodology involving a systematic
-study of designing, developing and evaluating online support tool for biodiversity
-training. Subjects of this study were selected from forest engineers that work within
-General Directory of Forestry. Purposive sampling method was conducted. Quality of web based learning was ensured by relying the development to Demand-Driven
-Learning Model as a theoretical framework.
-The results of the survey questions, interview sessions and system logs revealed that the
-perceptions of the participants towards the designed and developed tool were mostly
-positive. In addition, learners reported that they gain novel knowledge from training
-program, which they will reflect to their professional life, and find the training tool
-convenient. Moreover, their attitudes towards the all characteristics of theoretical
-framework were mostly positive. Findings also indicated that perceptions of the
-participants towards online training programs have changed as well.
-Keywords: Design and development research, demand driven learning model, 
-biodiversity training</v>
+	  The aim of this study was to design a guiding resource material about biodiveristy for Biology teachers. A total of 37 volunteer biology teachers serving in the central towns of Ankara Province participated in the study as the sampling group and commented on the resource material and biodiversity teaching. Interview method was used in the study.`Level of biodiversity knowledge? and `qualification perceptions of teachers? biodiversity education? were investigated by taking sex, years of service, type of school they are working at, average number of students in classes and faculty graduated, and determined using X2 (Chi-square test). The relationship between qualification perceptions of teachers? biodiversity education and their Level of biodiversity knowledge was found to be statistically significant.As the conclusion of this study, fifteen teachers who proposed suggestions about teaching biodiversity, emphasized the importance of applied education. Twenty one of the teachers participating in the study found the resource material of high quality, and 17 of them reported that the material increased their level of knowledge.The guiding resource material about biodiveristy can be reached via e-mail of the reasearcher at the adress: mineseckinkurumlu @gmail.com</v>
       </c>
     </row>
     <row r="7" xml:space="preserve">
@@ -696,16 +653,16 @@
       </c>
       <c r="H8" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	 Dünya biyoçeşitliliğinde (biyolojik çeşitliliğinde)  görülen azalma, insanların sorumsuzca faaliyetleri sonucu her geçen gün biraz daha tehlikeli boyutlara ulaşmaktadır. Bu durum biyoçeşitliliğin küresel çapta önem kazanmasına sebep olmuştur. Günümüzde biyoçeşitliliğin korunması, öğrenilmesi ve sürdürülebilirliğine yönelik ulusal ve uluslararası düzeyde çok önemli araştırmalar yapılmaktadır. Biyoçeşitlilikle ilgili var olan sorunların üstesinden gelebilmek için yapılan bu araştırmaların önemli bir kısmını öğretmen ve öğretmen adaylarıyla yapılan çalışmalar oluşturmaktadır.       
-Bu çalışma, öğretmenlerin biyoçeşitlilik konusundaki görüşlerini öğrenmek, çalıştığı bölgelerin biyoçeşitliliğini bilme ve bunu derslerinde işleme durumlarını belirlemek için hazırlanmış disiplinler arası bir çalışmadır. Çalışma grubunu Sakarya ili ve ilçelerinde görev yapmış üç biyoloji, üç coğrafya, üç fen bilimleri, üç sosyal bilgiler olmak üzere toplam on iki gönüllü öğretmen oluşturmaktadır. Nitel yaklaşım ekseninde hazırlanan bu fenomenolojik çalışmada yarı yapılandırılmış görüşme formu kullanılarak veriler toplanmıştır. Elde edilen veriler, içerik analizi yöntemi kullanılarak yorumlanmıştır. Verilen kodlanmasında NVİVO nitel veri analiz yazılımı kullanılmıştır. 
-Bu çalışma sonucunda ilgili branş öğretmenlerin biyoçeşitlilik konusunda eksikleri olduğu, çalıştığı bölgeleri yeterince araştırmadığı ancak biyoçeşitliliğin öneminin farkında oldukları fark edilmiştir. Ayrıca ilgili branş öğretmenlerinin biyoçeşitliliği öğrencilere aktarma konusunda yalnız kaldıkları, bu konuda medyadan, sivil toplum kuruluşlarından, devlet politikalarından, üniversitelerden, meslektaşlarından yeterince destek alamadıkları ifade edilmiştir. Müfredatta yeterince zaman ayrılmadığı için biyoçeşitlilik konusunun çok verimli işlenemediği anlaşılmıştır. Öğretmenlerden alınan görüşler doğrultusunda biyoçeşitliliğin verimli işlenebilmesi için gezi ve sergilerin düzenlenmesi, eğitim kamplarının yapılması, alanında uzman kişilerce okullarda seminer verilmesi, hayvanat bahçesi ve müze ziyaretlerinin yeterince önemsenmesi gerektiği gibi etkinlikler ifade edilmiştir. Çalışma sonucunda ayrıca toplumun da biyoçeşitlilik konusunda bilinçlenmesine yönelik eğitim faaliyetlerinin düzenlenmesi ve aile düzeyinde çalışmalar yapılması gerektiği anlaşılmıştır.
+	 Bu çalışmanın amacı 5, 6, 7 ve 8. sınıflarda okuyan öğrencilerin yakın çevrelerinde bulanan biyoçeşitlilik ile ilgili farkındalık düzeylerinin incelenmesidir. 
+Araştırmanın örneklemi 2015-2016 eğitim öğretim yılında Antalya ilinde okuyan 460 öğrenciden oluşmaktadır. Çalışmada 16 adet orijinaline uygun, baskı ve renk kalitesi yüksek, Antalya bölgesinde yetişen bitki resmi ile doğal yaşam alanı yine Antalya bölgesi olan 16 adet hayvan resmi 2 farklı A4 yaprağı üzerinde olacak şekilde öğrencilere dağıtılmıştır. Öğrencilerden bitki ve hayvan resimlerinin karşısında bırakılan boşluğa biliyorlarsa bu bitki ve hayvanların isimlerini yazmaları istenmiştir. Yapılan anketin hayvanlarla ilgili kısmında çıkan sonuca göre öğrencilerin biyoçeşitlilik konusundaki farkındalıklarının erkek öğrencilerde kız öğrencilere göre daha yüksek olduğu, bitkilerle ilgili kısmında çıkan sonuca göre ise erkek ve kız öğrenciler arasında anlamlı bir farklılık olmadığı tespit edilmiştir. Öğrencilerin biyoçeşitlilik konusundaki farkındalıklarına anne ve baba eğitiminin, ailenin gelir düzeyinin, öğrencinin doğa ile ilgili bir televizyon programı takip etmesinin istatistiksel olarak etkili olmadığı görülmüştür. Buna rağmen evde hayvan besleyen öğrencilerin beslemeyenlere göre hayvanları tanıma düzeylerinin daha yüksek olduğu tespit edilmiştir. 
+Elde edilen veriler ışığında öğrencilere çevre ve biyoçeşitlilik eğitimi verilirken; öğrencinin çevre ile direkt ilişki içinde olması, yaparak –yaşayarak öğrenmesi gerekmektedir. Öğrencilerin kendi bitkilerini yetiştirmelerinin, doğanın içinde bitkilerle ve hayvanlarla karşılaşmalarının, hayvan beslemelerinin onların zaman içinde biyoçeşitlilik kavramını daha iyi anlamalarına yardımcı olacağı düşünülmektedir.
 	 </v>
       </c>
       <c r="I8" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	  The reduction in world biodiversity is becoming more dangerous day by day as a result of people's irresponsible activities. This situation has caused the biodiversity to gain global importance. Today, very important researches are carried out at national and international level in order to protect, learn and sustain biodiversity. In order to overcome the existing problems related to biodiversity, a significant part of these researches consisted of studies conducted with teacher and teacher candidates.
-This study is an interdisciplinary study designed to learn teachers' views on biodiversity, to know the biodiversity of the regions where they work and to determine their status in their lessons. The study group consisted of three volunteer biology, three geography, three science and three social studies teachers worked in Sakarya and its districts. In this phenomenological study prepared on the basis of qualitative approach, data were collected using semi-structured interview form. The data were interpreted by using the content analysis method. NVİVO qualitative data analysis software was used in the given coding.
-As a result of this study, it was realized that the teachers in the related field had deficiencies in biodiversity, did not investigate sufficiently the regions where they work but they were aware of the importance of biodiversity. In addition, it was stated that the related branch teachers were alone in transferring the biodiversity to the students and they could not get enough support from the media, civil society organizations, state policies, universities and colleagues. It was noticed that biodiversity could not be processed very efficiently, because there was not enough time in the curriculum. According to the opinions taken from the teachers, it was stated that activities such as organizing trips and exhibitions, organizing training camps, giving seminars in schools to the experts in the field and the visits of the zoo and museums were necessary for efficient processing biodiversity. As a result of the study, it was understood that education activities should be organized in order to increase awareness of the society on biodiversity and studies should be carried out at family level.</v>
+	  The purpose of this study is to examine the levels of 5th 6th 7th and 8th grade students' awareness of the biodiversity in the immediate environment around them.
+The sample is consists of 460 students studying in Antalya in 2015-2016 education year. 16 authentic, high quality and high resolution pictures of plants growing in Antalya region and 16 pictures of animals, whose natural habitat is Antalya Region were handed out to the students on two seperate sheets of A4 paper. Students were asked to write the names of the animals and plants next to the pictures. According to the result of the survey regarding the animals, the awareness of the boys is higher than those of girls' and there has been no significiant difference in awarness with regards to plants among boys and girls. It has been observed that the educational level of students' parents, their income level and students' following a TV programme about natüre do not statistically affect students' awareness of the biodiversity. Despite this, it has been established that the students who have pets are better able to recognize animals than those who don't.
+In the light of the data gathered, the students must be in direct contact with the enviroment and learn by donig while they are being given education on enviroment and biodiversity. It is reasoned that students' growing their own plants, coming across plants and animals in nature and having a pet will help them understand the concept of biodiversity much better.</v>
       </c>
     </row>
     <row r="9" xml:space="preserve">
@@ -799,38 +756,6 @@
         <v>Eğitim ve Öğretim = Education and Training</v>
       </c>
       <c r="H11" t="str" xml:space="preserve">
-        <v xml:space="preserve"> 
-	 Araştırmanın amacı, ortaöğretim öğrencilerinin biyoçeşitliliğe yönelik bilgi, davranış ve tutumlarını ölçmektir. Araştırma, ortaöğretim öğrencilerinin biyoçeşitliliğe yönelik bilgi, davranış ve tutumlarını farklı değişkenler açısından belirlemeyi amaçladığından bu araştırmada betimsel tarama modelinde ilişkisel tarama yöntemi kullanılmıştır. Araştırmanın çalışma grubunu 2018-2019 eğitim öğretim yılında Ankara ilinde ortaöğretim kurumlarında okuyan 9, 10, 11, 12. sınıf öğrencileri oluşturmuştur. Araştırmada veriler, araştırmacı tarafından geliştirilen biyoçeşitlilik başarı testi, biyoçeşitlilik davranış ölçeği, biyoçeşitlilik tutum ölçeği ile toplanmıştır. Ölçek Ankara ilinde Milli Eğitim Bakanlığı'na bağlı okullarda 245 kişiye uygulanmıştır. Verilerin analizi için SPSS paket veri programı kullanılmıştır. Araştırma sonucunda, kız öğrencilerin biyoçeşitliliğe yönelik davranış ve tutumlarının erkek öğrencilere göre anlamlı düzeyde yüksek olduğu, biyoçeşitlilik başarı testi bakımından cinsiyete göre anlamlı bir farklılık olmadığı sonucuna ulaşılmıştır. Öğrencilerin çevreyle ilgili bir kulübe üye olmalarının biyoçeşitlilik okuryazarlığına etkisi olmadığı görülmüştür. Sınıf düzeyine göre öğrencilerin başarı ve tutumlarında anlamlı bir farklılık belirlenmiştir.
-	 </v>
-      </c>
-      <c r="I11" t="str" xml:space="preserve">
-        <v xml:space="preserve"> 
-	  The aim of the study is to qualify the knowledge, behavior and attitudes of secondary school students towards biodiversity. Since the research aimed to determine the knowledge, behavior and attitudes of secondary school students towards biodiversity in terms of different variables, relational scanning method was used in this descriptive scanning model. The 9th, 10th, 11th, 12th graders of secondary schools in Ankara created the team of this study in the 2018-2019 academic year. In this study all the data like biodiversity achievement test, biodiversity behavior scale and biodiversity attitude scale were collected by the analyst. The scale was applied to 245 people in schools affiliated to the Ministry of National Education in Ankara. The data program SPSS was used for data analysis. As a result of the study, it was concluded that female students' behaviors and attitudes towards biodiversity were significantly higher than male students and there were no significant differences towards biodiversity achievement test according to gender. It was observed that students' membership in an environmental club did not affect biodiversity literacy. A significant difference was determined towards achievement and attitudes of students according to their grade level.</v>
-      </c>
-    </row>
-    <row r="12" xml:space="preserve">
-      <c r="A12" t="str">
-        <v>13</v>
-      </c>
-      <c r="B12" t="str">
-        <v>290726</v>
-      </c>
-      <c r="C12" t="str">
-        <v>HATİCE ESRA GÜNAYDIN</v>
-      </c>
-      <c r="D12" t="str">
-        <v>2011</v>
-      </c>
-      <c r="E12" t="str">
-        <v>Bitkiler ve biyoçeşitliliğin öğretilmesine yönelik bir rehber materyal geliştirme çalışmasıA study on development a resource material for teaching plants and biodiversity</v>
-      </c>
-      <c r="F12" t="str">
-        <v>Yüksek Lisans</v>
-      </c>
-      <c r="G12" t="str">
-        <v>Biyoloji = Biology ; Eğitim ve Öğretim = Education and Training</v>
-      </c>
-      <c r="H12" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
 	 Biyolojik çeşitlilik, dünyada ilk canlının ortaya çıkışından bu yana oluşan çok değerli bir birikimdir. Bu birikim dünyanın yaşadığı değişmeler karşısında dengelerin yeniden kurulmasına olanak veren bir zenginliktir. Bu nedenle biyoçeşitliliğin varlığı gelecek nesiller için büyük önem taşımaktadır. Gelecek nesillerin biyoçeşitliliği oluşturan canlı türlerini, ekosistemleri tanıyabilmeleri için biyoçeşitliliğin korunması önemlidir. Bu nedenle bu çalışmada biyoçeşitliliğin neden ve nasıl korunması gerektiği irdelenmiştir. 
 Biyolojik çeşitliliğin korunabilmesi için biyopolitikaların olması gereklidir. Biopolitika'nın gereklerinin sağlanabilmesi için biyokültür kavramına ihtiyaç duyulmuştur. Biyokültür, biyoeğitimle sağlanabilir. Davranışların ahlaki ve sorumluluk boyutu biyoetik ile gerçekleştirilebilir (Arvanitis, 1989).
@@ -839,7 +764,7 @@
 Araştırmanın sonuçlarına göre, öğrencilerin biyoçeşitlilik konusu işlenmeden önceki test puanları, konu işlendikten sonraki test puanlarına göre anlamlı bir şekilde yüksektir. Kız öğrenciler hem ön testte hem de son testte erkek öğrencilerden daha yüksek puan almışlardır. İnternet'i kullanan öğrenciler ile internet'i kullanmayan öğrencilerin ön test ve son test puanlarında farklılık bulunmaktadır. İnternet'i kullanan öğrencilerin ön test ve son test puanları kullanmayan öğrencilere göre daha yüksektir. Bu sonuçlara göre internet'in öğrencilerin öğrenme süreçlerine dahil edilmesi önerilmektedir. Gelecek nesiller düşünüldüğünde, kız öğrencilerin okuması desteklenmelidir. MEB'e öğrencilerde biyoçeşitlilik kavramı ve önemi ile ilgili bilincin nasıl daha iyi oluşturulabileceği ve kavratılabileceği yönünde önerilerde bulunulmuştur.
 	 </v>
       </c>
-      <c r="I12" t="str" xml:space="preserve">
+      <c r="I11" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
 	  Biological diversity, which is an accumulation in the world since the emergence of the first living that occurs, is very valuable. This accumulation is a richness that allows re-establishment of stability in the face of change. Hence the presence of biodiversity is of great importance for future generations. Conservation of biodiversity is important for future generations for them to know biodiversity that consists of the living species and ecosystems. Therefore, the reasons for protection of biodiversity and ways to protect biodiversity is discussed in this study. 
 Biopolitics is needed for preservation of biological diversity. Bioculture concept is needed to achieve the requirements of Biopolitics. Bioculture can only be ensured through bioeducation. The moral and responsibility dimensions of behavior can be performed by bioethics (Arvanitis, 1989).
@@ -848,6 +773,46 @@
 According to the survey, test scores of students before the biodiversity chapter is studied are significantly higher comparing to the test results after biodiversity chapter is studied. Female students scored higher than male students in both pre-test and post-test. Pre-test and post-test scores of students who use internet are higher than those who do not use internet. Regarding these results, internet is proposed to be included in the student's learning process. Female students should be encouraged to study considering the future generations. Student awareness about the importance of biodiversity and how the concept can be created and comprehended is suggested to Ministry of Education.</v>
       </c>
     </row>
+    <row r="12" xml:space="preserve">
+      <c r="A12" t="str">
+        <v>13</v>
+      </c>
+      <c r="B12" t="str">
+        <v>290726</v>
+      </c>
+      <c r="C12" t="str">
+        <v>HATİCE ESRA GÜNAYDIN</v>
+      </c>
+      <c r="D12" t="str">
+        <v>2011</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Bitkiler ve biyoçeşitliliğin öğretilmesine yönelik bir rehber materyal geliştirme çalışmasıA study on development a resource material for teaching plants and biodiversity</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Yüksek Lisans</v>
+      </c>
+      <c r="G12" t="str">
+        <v>Biyoloji = Biology ; Eğitim ve Öğretim = Education and Training</v>
+      </c>
+      <c r="H12" t="str" xml:space="preserve">
+        <v xml:space="preserve"> 
+	 Biyolojik çeşitlilik, dünyada ilk canlının ortaya çıkışından bu yana oluşan çok değerli bir birikimdir. Bu birikim dünyanın yaşadığı değişmeler karşısında dengelerin yeniden kurulmasına olanak veren bir zenginliktir. Bu nedenle biyoçeşitliliğin varlığı gelecek nesiller için büyük önem taşımaktadır. Gelecek nesillerin biyoçeşitliliği oluşturan canlı türlerini, ekosistemleri tanıyabilmeleri için biyoçeşitliliğin korunması önemlidir. Bu nedenle bu çalışmada biyoçeşitliliğin neden ve nasıl korunması gerektiği irdelenmiştir. 
+Biyolojik çeşitliliğin korunabilmesi için biyopolitikaların olması gereklidir. Biopolitika'nın gereklerinin sağlanabilmesi için biyokültür kavramına ihtiyaç duyulmuştur. Biyokültür, biyoeğitimle sağlanabilir. Davranışların ahlaki ve sorumluluk boyutu biyoetik ile gerçekleştirilebilir (Arvanitis, 1989).
+Günümüzde okullarda verilen biyolojik çeşitlilik eğitimi incelendiğinde, biyolojik çeşitliliğin kavram olarak ilk kez ilköğretim 7. sınıflarda Fen ve Teknoloji dersi kapsamında işlendiği görülmektedir.  
+Bu bağlamda, araştırma kapsamında ilköğretim 7. Sınıf öğrencilerinin biyoçeşitlilik bilgilerini etkileyen faktörler ile MEB tarafından ilköğretim 7. Sınıf düzeyi için belirlenen öğretim programının öğrencilere biyoçeşitliliği kavratmada ve biyoçeşitlilik ile ilgili bilinç oluşturmada yeterli olup olmadığı incelenmiştir. Ayrıca bu konuyla ilgili öğretmenlerinde görüşleri alınmıştır. Araştırma kapsamında Ankara İlinde 5 ilköğretim okulunda öğrenim gören 412 7. sınıf öğrencisi ve bu okullarda görev yapan 12 fen ve teknoloji dersi öğretmeni ile görüşülerek anket çalışması ile veriler toplanmıştır. 
+Araştırmanın sonuçlarına göre, öğrencilerin biyoçeşitlilik konusu işlenmeden önceki test puanları, konu işlendikten sonraki test puanlarına göre anlamlı bir şekilde yüksektir. Kız öğrenciler hem ön testte hem de son testte erkek öğrencilerden daha yüksek puan almışlardır. İnternet'i kullanan öğrenciler ile internet'i kullanmayan öğrencilerin ön test ve son test puanlarında farklılık bulunmaktadır. İnternet'i kullanan öğrencilerin ön test ve son test puanları kullanmayan öğrencilere göre daha yüksektir. Bu sonuçlara göre internet'in öğrencilerin öğrenme süreçlerine dahil edilmesi önerilmektedir. Gelecek nesiller düşünüldüğünde, kız öğrencilerin okuması desteklenmelidir. MEB'e öğrencilerde biyoçeşitlilik kavramı ve önemi ile ilgili bilincin nasıl daha iyi oluşturulabileceği ve kavratılabileceği yönünde önerilerde bulunulmuştur.
+	 </v>
+      </c>
+      <c r="I12" t="str" xml:space="preserve">
+        <v xml:space="preserve"> 
+	  Biological diversity, which is an accumulation in the world since the emergence of the first living that occurs, is very valuable. This accumulation is a richness that allows re-establishment of stability in the face of change. Hence the presence of biodiversity is of great importance for future generations. Conservation of biodiversity is important for future generations for them to know biodiversity that consists of the living species and ecosystems. Therefore, the reasons for protection of biodiversity and ways to protect biodiversity is discussed in this study. 
+Biopolitics is needed for preservation of biological diversity. Bioculture concept is needed to achieve the requirements of Biopolitics. Bioculture can only be ensured through bioeducation. The moral and responsibility dimensions of behavior can be performed by bioethics (Arvanitis, 1989).
+Today, when the scope of biodiversity education is examined, biodiversity concept is first seen in the scope of Science and Technology course of 7th grades. 
+In this context, the scope of research 7th Students with the Ministry of factors affecting biodiversity information 7th by Specified for the grade level curriculum to students to create awareness about biodiversity and biodiversity In comprehend examined whether there was adequate. We also sought the views of teachers on this issue. Scope of research studying in primary schools in Ankara Province 5 412 7 Students and those who work in schools with 12 teachers of science and technology courses in consultation with survey data was collected.
+According to the survey, test scores of students before the biodiversity chapter is studied are significantly higher comparing to the test results after biodiversity chapter is studied. Female students scored higher than male students in both pre-test and post-test. Pre-test and post-test scores of students who use internet are higher than those who do not use internet. Regarding these results, internet is proposed to be included in the student's learning process. Female students should be encouraged to study considering the future generations. Student awareness about the importance of biodiversity and how the concept can be created and comprehended is suggested to Ministry of Education.</v>
+      </c>
+    </row>
     <row r="13" xml:space="preserve">
       <c r="A13" t="str">
         <v>19</v>
@@ -872,12 +837,14 @@
       </c>
       <c r="H13" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	 Bu çalışma, bitkiler ve biyoçeşitliliğin öğretilmesine yönelik bir rehber materyal geliştirmek amacıyla yapılmıştır. Araştırmada görüşme yöntemi kullanılmış, Ankara ili merkez ilçelerinde görev yapmakta olan 22 biyoloji öğretmeninin hazırlanan rehber materyal ve biyoçeşitlilikle ilgili görüşleri alınmıştır.Araştırmanın sonucunda, öğretmenlerin biyoçeşitlilik konusunda hâkimiyet düzeylerinin yeterli olmadığı; biyoçeşitlilik konusundaki bilgi düzeylerini tanımlayabildikleri tür sayısıyla eş değer tuttukları tespit edilmiştir. Öğretmenler, öğrencilerinin de konuyla ilgili bilgi seviyelerinin yeterli olmadığını belirtmiş, bunun nedeni olarak ise ilköğretimde konuya yeterli ağırlılık verilmemesini göstermişlerdir. Öğretmenlerin rehber materyal kullanımına yeterli önemi vermedikleri, biyoçeşitlilik konusunu yüzeysel bir anlatımla geçtikleri ise araştırmada ortaya çıkan bir diğer sonuçtur. Müfredatta biyoçeşitlilik konusunun öğrenci seviyesinde ele alınmasına rağmen, konuyu tam olarak kavratmada yetersiz kaldığı; uygulama ve görsellikte eksiklerinin olduğu da araştırmanın çıktılarından biridir.Araştırmacı tarafından hazırlanan rehber materyal öğretmenlerin tümü tarafından beğenilmiş, öğretici bir nitelik taşıdığı belirtilmiştir.
+	 Bu çalışmada amaç; "Canlılar ve Yaşam" öğrenme alanı içerinde yer alan canlıların sınıflandırılması, biyoçeşitlilik ve yıkıcı doğa olayları kavramlarına yönelik geliştirilen aktif öğrenme teknikleri ile zenginleştirilmiş çalışma yapraklarının hafif düzeyde zihinsel yetersizliği olan kaynaştırma öğrencilerinin ve normal gelişim gösteren öğrencilerin bilimsel süreç beceri gelişimi ve kavramsal anlamaları üzerine etkisini ortaya çıkarmaktır. Araştırmada karma yöntemden yararlanılmıştır. Çalışmanın örneklemini; beşinci sınıfta öğrenim gören 16 (sekiz hafif düzeyde zihinsel yetersizliği olan ve sekiz normal gelişim gösteren) öğrenci oluşturmaktadır. Asıl uygulamada iki ayrı grup oluşturulup çalışılmıştır. Birinci grup hafif düzeyde zihinsel yetersizliği olan sekiz öğrenciden, ikinci grup ise normal gelişim gösteren sekiz öğrenciden oluşmaktadır. Pilot uygulama 4 öğrenci ile yürütülmüştür. Pilot uygulama 2018-2019 ve asıl uygulama 2019-2020 eğitim-öğretim yıllarında yapılmıştır. Tahmin-Gözlem-Açıklama (TGA) yönteme uygun hazırlanan çalışma yaprakları; dikkat çekme-etkin uğraşı ve değerlendirme bölümlerinden oluşmaktadır. TGA yöntemi içerisinde aktif öğrenme tekniklerinden (vızıltı 22-öğrenme galerisi-kart gösterme-kartopu) ve mobil öğrenme (karekod uygulaması) uygulamalarından yararlanılmıştır. Çalışmada veri toplama aracı olarak; "Canlılar ve Yaşam" öğrenme alanında ilgili kavramlar için geliştirilen Bilimsel Süreç Beceri Gelişim (BiSBeG) formu ve görüşme sorularından yararlanılmıştır. Canlıların sınıflandırılması, biyoçeşitlilik, yıkıcı doğa olayları kavramlarına yönelik üç çalışma yaprağı geliştirilmiştir. Araştırma sonucunda; "Canlılar ve Yaşam" öğrenme alanı içerinde yer alan canlıların sınıflandırılması, biyoçeşitlilik, yıkıcı doğa olayları kavramlarına yönelik aktif öğrenme teknikleri ile zenginleştirilmiş TGA yönteminin entegre edildiği çalışma yapraklarının hafif düzeyde zihinsel yetersizliğe sahip kaynaştırma öğrencilerinin ve normal gelişim gösteren öğrencilerin bilimsel süreç beceri gelişimleri üzerinde olumlu etkide bulunduğu sonucuna varılmıştır (z=2,533, p&lt;.05; z=2,521, p&lt;.05). Aktif öğrenme teknikleri ile zenginleştirilmiş çalışma yapraklarının sınıfında hem "hafif düzeyde zihinsel yetersizliği" hem de "normal gelişim gösteren" öğrencileri bulunan öğretmenlerce kullanılarak, öğrencilerin bilimsel süreç becerilerini ve kavramsal anlamalarını geliştirebileceği düşünülmektedir.
+Anahtar Kelimeler: Hafif Düzeyde Zihinsel Yetersizlik, Bilimsel Süreç Becerileri, Tahmin-Gözlem-Açıklama, Aktif Öğrenme Teknikleri, Canlılar ve Yaşam.
 	 </v>
       </c>
       <c r="I13" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	  The aim of this study was to design and develop a resource material for teaching plants and biodiversity. During the research, interview method was used and opinions of 22 biology teachers working in central districts of Ankara were obtained on the developed biodiversity resource material.Results of the study showed that the teachers levels of expertise/command on biodiversity were not satisfactory and that they envisoned their level of knowledge on biodiversity with the number of species could identify. Teachers also indicated that the students? levels of knowledge on the subject were not sufficient and claimed the reason to the little weight given to the subject in primary school education. Another result of the study was that teachers did not give necessary importance to using resource materials and carried out teaching activities with a superficial teaching approach. Although the subject of biodiversity is present at the students? level in the curriculum, it was inefficient to completely comprehend the subject, lacked practice and visual components.The resource material prepared by the researcher was appreciated by all participating teachers and they commented that the material was of teaching/instructive quality.</v>
+	  The purpose of this study; is to uncover the effect of worksheets enriched with active learning techniques developed for the concepts of classification of living things, biodiversity and destructive natural events in the "Living Beings and Life" learning area on the scientific process skill development and conceptual understanding of inclusive students with mild intellectual disability and students with normal development. The mixed method was used in the research. Participated in the study; there are 16 students (eight with mild mental disabilities and eight with normal development) who are studying in the fifth grade. In the actual application, two separate groups have been created and studied. The applications were conducted in a single school with eight students in the second group. The pilot application was conducted with 4 students. The pilot application was conducted in 2018-2019 and the actual application was conducted in 2019-2020 academic years. The worksheets prepared in accordance with the Prediction-Observation-Explanation (POE) method consist of attention-seeking-effective engagement and evaluation sections. Active learning techniques (buzz 22-learning gallery-card display-snowball) and mobile learning (karekod application) applications were used within the POE method. As a data collection tool in the study; The Scientific Process Skill Development (BiSBeG) form developed for related concepts in the field of learning "Living Things and Life" and interview questions were used. Three sheets of work have been developed on the concepts of classification of living beings, biodiversity, destructive natural phenomena. As a result of the research; "Living life and learning" situated in the area of living things classification, biodiversity, the concepts of destructive natural events-oriented active learning techniques enriched with students with mild mental impairment POE method is the integrated study of the inclusion of students with normal development of the leaves ' came to the conclusion that had a positive impact on the development of science process skills (z=2,533, p&lt;.05; z=2,521, p&lt;,05). It is thought that using the worksheets enriched with active learning techniques by the teachers who have both "mild intellectual disability" and "normally developing" students in their classrooms can improve students' scientific process skills and conceptual understanding.
+Keywords: Mild Mental Disabilities, Skill Development, Prediction-Observation-Explanation Worksheet, Active Learning Techniques</v>
       </c>
     </row>
     <row r="14" xml:space="preserve">
@@ -937,38 +904,6 @@
         <v>Eğitim ve Öğretim = Education and Training</v>
       </c>
       <c r="H15" t="str" xml:space="preserve">
-        <v xml:space="preserve"> 
-	 Bu çalışma "Canlılar Dünyasını Gezelim ve Tanıyalım" ünitesi çerçevesinde yapılan formal ve informal uygulamaların öğrencilerin çevre bilgi düzeyi ve çevreye yönelik tutumları üzerindeki etkisinin saptanması ve bilişsel-duyuşsal kazanımlarının ortaya çıkartılması amacıyla yapılmıştır. Çalışma, Samsun il merkezinde yer alan bir devlet okulu ile bir özel okul ve köyde yer alan bir devlet okulunda gerçekleştirilmiştir.  Her okuldan bir kontrol ve bir deney grubu olmak üzere ikişer sınıf seçilmiştir. Çalışmada, deney gurubunda il merkezindeki devlet okulundan 21, özel okuldan 19, köy okulundan 20 ve kontrol grubunda ise il merkezindeki devlet okulundan 20, özel okuldan 19 ve köy okulundan 17 olmak üzere toplam 116 öğrenci yer almıştır. Nicel ve nitel verilerin elde edildiği karma yöntemle yürütülen araştırmanın nicel verileri SPSS paket programı ile analiz edilmiş, nitel verilerin analizinde ise içerik analizi yapılmıştır. Nicel veri toplama aracı olarak "Çevreye Yönelik Bilgi Testi", "Çevreye Yönelik Tutum Ölçeği" kullanılmış ve nitel veri toplama aracı olarak "Çevre Eğitimi Uygulamaları Değerlendirme Formu", "Mülakatlar", "Çevre Gözlem Sınıflandırma Kağıtları", ve "Araştırmacı Genel Gözlem Formu" kullanılmıştır. Nicel olarak çevreye yönelik bilgi testinden elde edilen sonuçlara bakıldığında sadece köyde yer alan devlet okulu öğrencilerinin deney ve kontrol grupları arasında çevre bilgisi bakımından deney grubunun lehine anlamlı farklılık görülürken, il merkezinde yer alan devlet okulu ve özel okul öğrencilerinde deney ve kontrol grupları arasında anlamlı bir farklılık görülmemiştir. Okulların deney grubu öğrencilerinin karşılaştırılmasında ise köyde yer alan devlet okulunun il merkezinde yer alan devlet okulu ve özel okula göre çevre bilgi düzeylerinde daha fazla gelişme olduğu görülmüştür. Çevreye yönelik tutumlar incelendiğinde her üç okulun öğrencilerinde deney ve kontrol grupları arasında herhangi bir anlamlı farklılık görülmemiştir. Okulların deney grubu öğrencilerinin karşılaştırılmasında ise özel okul öğrencilerinin il merkezinde yer alan devlet okulu öğrencilerine göre çevreye yönelik tutumlarında olumlu yönde gelişim olduğu gözlenmiştir. Buna göre; doğal yaşama daha yakın olan öğrencilerin formal ve informal öğrenmelerinin birlikte desteklendiği durumlarda çevreye yönelik bilgilenmeleri açısından daha başarılı sonuçlar elde ettikleri, doğal yaşamdan uzak olan öğrencilerin ise çevreye yönelik tutum açısından olumlu yönde daha çok farklılaştığı sonucuna varılmıştır. Nitel olarak "Çevre Eğitimi Uygulamaları Değerlendirme Formu"ndan elde edilen sonuçlara göre; çevre eğitimine yönelik formal ve informal uygulamaların öğrencilerde meydana getirdiği bilişsel ve duyuşsal kazanımlar tespit edilmiştir. Buna göre; öğrencilerin bilişsel kazanımlarının "Doğa ve Canlılar", "Çevre Sorunları ve Çözümü" ve "Yaşam" konularında olduğu saptanmıştır. Duyuşsal kazanımların ise, "Doğa ve Canlılarla Etkileşim ve Öğrenme", "Çevre Koruma" ve " Sosyal İletişim ve Öğrenme" konularında olduğu tespit edilmiştir. Çevre eğitimine yönelik yapılan formal ve informal uygulamaların kazandırdığı bilişsel ve duyuşsal kazanımlar çevre konularında öğrenme zenginliği gerçekleştirilmesi ve yaşam boyu öğrenmeyi sürdürecek motivasyonun oluşturulması açısından önemli bir sonuç olmuştur. Mülakatlardan elde edilen sonuçlara bakıldığında; öğrencilerin tamamı etkinliklerle ilgili olumlu yönde görüş belirtmişlerdir. Öğrencilerin "Kuşlar, Kuş Halkalama", "Doğal Yaşam, Doğal Ortam", "Biyoçeşitlilik", "Atıkların Zararları ve Doğa Koruma", "Bitki Kurutma", "Canlı-Cansız Ayrımı ve Sınıflandırılma" ve "Canlıların Yaşam Ortamı" konularında öğrenmeler gerçekleştirdikleri belirlenmiştir. Öğrencilerin sınıfta öğrenilemeyen ancak çalışmada yer alan etkinliklerle öğrendiklerini belirttikleri konular ise "Kuşlar, Kuş Halkalama", "Atıklar", "Bitki kurutma", "Biyoçeşitlilik", "Doğal Yaşam Ortamları" ve "Doğada Çalışma" olmuştur. Gerçekleştirilen etkinliklerin öğrenciler tarafından beğenilerek doğada çalışma, öğrenme ve zaman geçirme isteğinin oluşması; biyoçeşitlilik, doğa ve doğanın korunması konularında öğrencilerin kendi öğrenmelerini yapılandırabilmeleri sağlanmıştır. Yapılan çalışma, öğretim programında yer alan kazanımların gerçek yaşam deneyimleri yolu ile kazandırılmasına ve öğrencilerin formal ve informal öğrenmelerini bütünleştirmelerine yol açmıştır. "Çevre Gözlem-Sınıflandırma Kâğıtları"ndan elde edilen sonuçlara göre öğrenciler ders kitaplarında yer almayan birçok canlı ve cansız varlığı gözlemlemişlerdir. Cansız varlıklardan yaşama ait kullanılanların, canlı varlıklardan ise günlük yaşamda sık karşılaşılanların daha çok yazıldığı görülmektedir. Öğrenciler tarafından yapılan sınıflandırmalarda günlük yaşamda sık karşılaşılan canlıların ve yaşamda kullanılan cansız varlıkların yazılmış olması nedeni ile fen derslerinde doğa ve canlılarla sık sık etkileşimin sağlanmasının tanıdık olunan varlıkların sayısında artışa neden olabileceği düşünülmüştür. Araştırmacı gözlemlerine göre ise "Doğada Öğrenmeye ve Zaman Geçirmeye Duyulan İlgi ve İstek durumu", Doğa ve Canlılara Karşı Tutum", "Gerçekleştirilen Öğrenmeler", "Etkinlikler Sırasında Eğitimciler ve Akranlarına Karşı Tutum" boyutlarında devlet okullarında biraz daha fazla olmak üzere her üç okulun benzer öğrenmeler gerçekleştirdikleri tespit edilmiştir. Küçük yaşlardan itibaren doğa ve canlılarla etkileşimin sağlanmasının, doğa ve canlılarla ilgili olumlu tutuma sahip olunması konusunda önemli bir durum olduğunu düşünmekteyiz. Tüm sonuçlar ele alındığında; formal ve informal uygulamaların birlikte kullanılması durumunda öğrenmenin, çevreye karşı olumlu tutum gelişiminin, bilişsel ve duyuşsal kazanımların daha fazla olabileceği sonucuna varılmıştır. Bu nedenle bu tür uygulamaların her sınıf düzeyinde ve birçok ünitenin öğretilmesinde yararlı olabileceği düşünülmektedir.
-	 </v>
-      </c>
-      <c r="I15" t="str" xml:space="preserve">
-        <v xml:space="preserve"> 
-	  This study examines the impacts of formal and informal practices within the "Exploring the World of Living Creatures" unit on the level of environmental information taken in students, and their approach to the environment, and assesses their cognitive and affective outcomes. The study involved the students of a state school and a private school in the center of Samsun, and a state school located in a village, with two classes chosen from each school to serve as an experiment group and a control group. The experiment group comprised 21 students from the state school in the city center, 19 students from the private school and 20 students from the village school, while and the control group comprised 20 students from the state school in the city center, 19 students from the private school and 17 students from the village school. In total, 116 students were involved in the study, in which both qualitative and quantitative data was analyzed. The quantitative data was analyzed using the SPSS package program, and the qualitative data was analyzed by way of a content analysis. The collection of quantitative data was made using the "Environmental Information Test" and the "Environmental Approach Scale", while the "Assessment Survey for Environment Education Practices", the "Interviews" the "Environmental Observation Classification Papers"  and the "Researcher General Observation Form" were employed for the collection of qualitative data. On the quantitative side, an analysis of the results from the Environmental Information Test revealed that only in the village school was there a significant difference between the experiment and the control groups in favor of the control group, in terms of garnered environmental information; while no significant differences were identified between the experiment and control groups in either the state school or private school located in the city center. A comparison of the experiment groups of the three schools reveals that students of the village school have a better level of environmental information than the students of both the state school and the private school in the city center. When we examined the approaches of the students toward the environment, no significant difference was observed between the experiment and control groups. When the students in the experiment group of each school were compared, private school students have improved their approach towards the environment better than the state school in the city center. Accordingly, it can be understood that students who live closer to nature retain more environmental information, as their formal and informal learning occur simultaneously, while students who live further away from nature experience a greater positive improvement in their attitude toward nature than the other students. Qualitatively, the results of the "Assessment Survey for Environment Education Practices" indicated that formal and informal practices in environment education had cognitive and affective outcomes in the students. Accordingly, it was determined that the students had cognitive outcomes in regards to "Nature and Living Creatures", "Solutions to Problems in Nature" and "Life", with affective outcomes noted in "Nature and Interaction with Living Things and Learning", "Environmental Conservation" and "Social Communication and Learning". The cognitive and affective outcomes related to formal and informal practices in environmental education are significant, since they enrich environmental learning and motivate the students toward life-long learning. When the results of the interviews were examined, all of the students commented positively on the events. It was determined that students learned about "Birds, Bird Banding", "Natural Life, Natural Environment", "Bio-diversity", "Harm done to the Environment and Living Creatures by Waste and Nature Conservation", "Drying Plants", "Living Non-Living Distinction and Classifying Living Creatures" and the "Habitats of Living Creatures". The students reported that "Bird Banding, Birds", "Wastes", "Drying Plants", "Bio-diversity", "Habitats" and "Studying in the Nature" were subjects that had not learned in the classroom, but learned during the events. The events gave the students a willingness to study, learn and spend time in nature, and to structure their own learning on bio-diversity, nature and nature conservation. These practices helped the students to learn about the subjects included in their curriculum with real life experiences, and to integrate their formal and informal learning. The results of the "Environmental Observation Classification Papers" indicated that the students observed many living and non-living things that are not included in their school books. It was seen that the students wrote mostly about non-livings things used in daily life, and the living creatures they encountered frequently in daily life. Since the students mostly wrote, in the classifications, the names of the living creatures they encountered frequently and the non-living things used in daily life, it is believed that frequent interactions with nature and living creatures may increase the number of the animals known by the students. According the researcher observations, all three schools demonstrated almost the same learning levels, although the two state schools recorded slightly higher levels, in the "Interest and Will to Learn and Spend Time in Nature", "Attitude Towards Nature and Living Creatures", "Learnings Performed" and "Attitude toward Instructors and Peers during the Events" areas. We believe that it is important for children to have the opportunity to interact with nature and living creatures so that they develop a positive approach to nature and living things. Considering all of the outcomes, it is concluded that the use of formal and informal practices together results in better learning, in the development of positive attitudes towards the environment, and better cognitive and affective outcomes. Accordingly, it is believed that making use of such practices will be beneficial in the teaching of many units among students of any grade.</v>
-      </c>
-    </row>
-    <row r="16" xml:space="preserve">
-      <c r="A16" t="str">
-        <v>25</v>
-      </c>
-      <c r="B16" t="str">
-        <v>454694</v>
-      </c>
-      <c r="C16" t="str">
-        <v>DURMUŞ YANMAZ</v>
-      </c>
-      <c r="D16" t="str">
-        <v>2017</v>
-      </c>
-      <c r="E16" t="str">
-        <v>Doğa tarihi müzesinde rehber hazırlama ve çalışma yaprakları ile öğretimin öğrencilerin akademik başarı ve fen öğrenimine yönelik motivasyonları üzerine etkisiInvestigating the effect of teaching with museum guide preparation and museum worksheets at natural history museum on students' academic success and motivation towards science learning</v>
-      </c>
-      <c r="F16" t="str">
-        <v>Yüksek Lisans</v>
-      </c>
-      <c r="G16" t="str">
-        <v>Eğitim ve Öğretim = Education and Training ; Müzecilik = Museology</v>
-      </c>
-      <c r="H16" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
 	 Bu çalışma Fen Bilgisi programında öğrenim gören öğretmen adaylarının yakın çevrelerindeki bitkilerini tanıma düzeyleri ve biyolojik çeşitlilik hakkında farkındalıklarını belirlemek amacıyla yürütülmüştür.
 Nitel bulguları nicel bulgularla destekleyen, fen alanı araştırmalarda da sıkça kullanılan karma araştırma yöntemi ve iki değişken arasındaki farklılığa bakılan karşılaştırmalı durum çalışması seçilmiştir. Araştırma belli bir amaç doğrultusunda yürütüldüğü içi amaçlı örneklem yöntemiyle çevreyle ilgili ders alan ve almayan öğretmen adayları seçilmiştir. Araştırma çevreyle ilgili ders almayan 1. ve 2. Sınıf öğretmen adayları ve çevreyle ilgili ders alan 3. ve 4. Sınıf öğretmen adaylarıyla yürütülmüştür. Çalışmada veriler iki şekilde toplanmıştır. Birinci kısımda yakın çevrelerindeki bitkilerini tanıma düzeyleri belirlemek için bir form kullanılmış ve bir istatistik programıyla nicel bulguları bulunmuştur. İkinci kısımda ise biyoçeşitlilik görüşme sorularıyla da öğretmen adaylarının biyoçeşitlilik ve çevre sorunlarına karşı daha detaylı incelemek için bir görüşme formu kullanılmıştır. Nicel bulgular istatistik programıyla, nitel bulgular ise içerik analiz yöntemiyle bulunmuştur.
@@ -977,7 +912,7 @@
 Çevre bilimi, evrim gibi dersleri alan öğrencilerin biyoçeşitlilik hakkında daha diğer düzeylere göre daha bilinçli oldukları ve 4. Sınıfların staj yapmalarından dolayı kendilerini bir öğretmen gibi hissettikleri ve öğrencilerin düzeyine uygun projeler geliştirdikleri sonucu çıkmıştır. 4. Sınıf öğretmen adayları alt kademedeki öğretmen adaylarına kıyasla çevre farkındalığı yüksektir ama bütün öğretmen adayları biyolojik çeşitlilik kavramını tür çeşitliliğiyle karıştırmışlardır. Buda aldığı derslerin olumlu yönde etki ettiği ama yeterli olmadığı sonucuna ulaşılmıştır.
 	 </v>
       </c>
-      <c r="I16" t="str" xml:space="preserve">
+      <c r="I15" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
 	  This study has been conducted to determine the awareness about biological varlety and the limitation of knowledge about plant recognition of science teacher candidates.
 Combined research method, which supports qualitative findings with quantitative findings while being widely used in science researches and comperative state study which focuses on the differences between two changeables have been chosen.Because the research is conducted for a spesific purpose, teacher candidates who take lessons about environment and those who do not have been chosen with purposeful sampling method. The research has been conducted with 1st and 2st year teacher candidates who do not get lectures on nature and 3 rd and 4 th year candidates who do. The data has been collected in two ways. İn the first part a form is given to assess their level of plant recognition and quantitative findings are received with a statistics programe. İn the second part an interview form is used to learn more about their stand on biovariety and enviromental issues with bio-diversity based questions. Quantitative findings are acquired with a statistics programe and qualitative findings are acquired by content analysis. 
@@ -985,6 +920,45 @@
 Another finding is that students who get lessons like "nature science" or "evolution" are better informed, moreover they feel more teacher-like because of their internship programe in the final year and therefore produce more age-appropriate projects for their students. Teacher candidates that study at their 4th year have higher enviromental awareness in comparison to lower grades but all candidates confused bio-diversity with kind-diversity, which made clear that the curriculum had a positive impact but not enough.</v>
       </c>
     </row>
+    <row r="16" xml:space="preserve">
+      <c r="A16" t="str">
+        <v>25</v>
+      </c>
+      <c r="B16" t="str">
+        <v>454694</v>
+      </c>
+      <c r="C16" t="str">
+        <v>DURMUŞ YANMAZ</v>
+      </c>
+      <c r="D16" t="str">
+        <v>2017</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Doğa tarihi müzesinde rehber hazırlama ve çalışma yaprakları ile öğretimin öğrencilerin akademik başarı ve fen öğrenimine yönelik motivasyonları üzerine etkisiInvestigating the effect of teaching with museum guide preparation and museum worksheets at natural history museum on students' academic success and motivation towards science learning</v>
+      </c>
+      <c r="F16" t="str">
+        <v>Yüksek Lisans</v>
+      </c>
+      <c r="G16" t="str">
+        <v>Eğitim ve Öğretim = Education and Training ; Müzecilik = Museology</v>
+      </c>
+      <c r="H16" t="str" xml:space="preserve">
+        <v xml:space="preserve"> 
+	 Bu çalışma Fen Bilgisi programında öğrenim gören öğretmen adaylarının yakın çevrelerindeki bitkilerini tanıma düzeyleri ve biyolojik çeşitlilik hakkında farkındalıklarını belirlemek amacıyla yürütülmüştür.
+Nitel bulguları nicel bulgularla destekleyen, fen alanı araştırmalarda da sıkça kullanılan karma araştırma yöntemi ve iki değişken arasındaki farklılığa bakılan karşılaştırmalı durum çalışması seçilmiştir. Araştırma belli bir amaç doğrultusunda yürütüldüğü içi amaçlı örneklem yöntemiyle çevreyle ilgili ders alan ve almayan öğretmen adayları seçilmiştir. Araştırma çevreyle ilgili ders almayan 1. ve 2. Sınıf öğretmen adayları ve çevreyle ilgili ders alan 3. ve 4. Sınıf öğretmen adaylarıyla yürütülmüştür. Çalışmada veriler iki şekilde toplanmıştır. Birinci kısımda yakın çevrelerindeki bitkilerini tanıma düzeyleri belirlemek için bir form kullanılmış ve bir istatistik programıyla nicel bulguları bulunmuştur. İkinci kısımda ise biyoçeşitlilik görüşme sorularıyla da öğretmen adaylarının biyoçeşitlilik ve çevre sorunlarına karşı daha detaylı incelemek için bir görüşme formu kullanılmıştır. Nicel bulgular istatistik programıyla, nitel bulgular ise içerik analiz yöntemiyle bulunmuştur.
+Araştırmanın bulgularında kızlarla erkekler arasında anlamlı bir fark görüldüğü ve sınıf düzeyleri arttıkça yakın çevrelerindeki bitkileri ve önemini de kavradıkları tespit edilmiştir. Öğretmen adaylarının çevreyle ilgili bilgi edindikleri yer internet iken; sınıf düzeyi arttıkça diğer yayın ve yayım organlarına başvurdukları görülmektedir. Öğretmen adayları biyolojik çeşitliliğin azalmasındaki en önemli faktöre toplumun bilinçsizce davranmasını söylerken, artması için ise ceza uygulaması ve topluma eğitim verilmesi gerektiğini söylemişlerdir. 
+Öğretmen adaylarının 3. Sınıfta aldıkları öğretim teknolojileri ve materyal dersi çevreyle ilgili proje yaparken öğretim materyalleri yapmak, eğitici oyunlar gibi öğretim yöntemleri öne sunmuşlardır.
+Çevre bilimi, evrim gibi dersleri alan öğrencilerin biyoçeşitlilik hakkında daha diğer düzeylere göre daha bilinçli oldukları ve 4. Sınıfların staj yapmalarından dolayı kendilerini bir öğretmen gibi hissettikleri ve öğrencilerin düzeyine uygun projeler geliştirdikleri sonucu çıkmıştır. 4. Sınıf öğretmen adayları alt kademedeki öğretmen adaylarına kıyasla çevre farkındalığı yüksektir ama bütün öğretmen adayları biyolojik çeşitlilik kavramını tür çeşitliliğiyle karıştırmışlardır. Buda aldığı derslerin olumlu yönde etki ettiği ama yeterli olmadığı sonucuna ulaşılmıştır.
+	 </v>
+      </c>
+      <c r="I16" t="str" xml:space="preserve">
+        <v xml:space="preserve"> 
+	  This study has been conducted to determine the awareness about biological varlety and the limitation of knowledge about plant recognition of science teacher candidates.
+Combined research method, which supports qualitative findings with quantitative findings while being widely used in science researches and comperative state study which focuses on the differences between two changeables have been chosen.Because the research is conducted for a spesific purpose, teacher candidates who take lessons about environment and those who do not have been chosen with purposeful sampling method. The research has been conducted with 1st and 2st year teacher candidates who do not get lectures on nature and 3 rd and 4 th year candidates who do. The data has been collected in two ways. İn the first part a form is given to assess their level of plant recognition and quantitative findings are received with a statistics programe. İn the second part an interview form is used to learn more about their stand on biovariety and enviromental issues with bio-diversity based questions. Quantitative findings are acquired with a statistics programe and qualitative findings are acquired by content analysis. 
+The findings suggest that there is a significant difference between male and female participants and that they realize more about the plants and their importance as their Education proceeds. While the source where candidate teachers learn about environment is the internet; it is recognized that they consult to other publishings and sources as their Education level increases.Candidates confuse the consept of bio-diversity with diversity of kind. While they use Education Technologies and material lesson which they are given in the 3rd year to create a project about the enviroment, they also presented other teaching methods like creating teaching methods and educational games. Prospective teachers stated that the reason why bio-diversity is decreasins is basıcally because the community is ignorant and that education and punishment is necessary for it to increase.
+Another finding is that students who get lessons like "nature science" or "evolution" are better informed, moreover they feel more teacher-like because of their internship programe in the final year and therefore produce more age-appropriate projects for their students. Teacher candidates that study at their 4th year have higher enviromental awareness in comparison to lower grades but all candidates confused bio-diversity with kind-diversity, which made clear that the curriculum had a positive impact but not enough.</v>
+      </c>
+    </row>
     <row r="17" xml:space="preserve">
       <c r="A17" t="str">
         <v>30</v>
@@ -1009,14 +983,12 @@
       </c>
       <c r="H17" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	 Non-formal öğrenme için uygun olan okul dışı öğrenme ortamları arasında  müzeler, bilim merkezleri, hayvanat bahçeleri, parklar, planetaryumlar vb. yer almaktadır. Müzeler fen eğitiminde yaygın olarak ziyaret edilen okul dışı öğrenme ortamlarından biridir. Özellikle doğa tarihi müzeleri fen eğitimi için oldukça uygundur. Çalışma yaprakları müzelerde fen eğitimi için yaygın olarak kullanılan öğretim stratejilerinden biridir. Müze çalışma yapraklarının etkililiği hakkında fikir ayrılıkları vardır. Müzelerde yeni öğretim stratejilerinin tasarlanmasına, uygulanmasına ve etkilerinin değerlendirilmesine ihtiyaç duyulmaktadır. Bu çalışmanın amacı; doğa tarihi müzesinde öğrencilerin müze rehberi hazırlaması yoluyla öğretim ve müze çalışma yaprakları yoluyla öğretimin, öğrencilerin fosil ve biyoçeşitlilik konularındaki fen başarıları ve fen öğrenimine yönelik motivasyonları üzerine etkilerini incelemek, kıyaslamak ve bu etkilerin kalıcılığını değerlendirmektir. Çalışma yarı deneysel yöntemlerden, eşitlenmemiş kontrol gruplu model olarak yürütülmüştür. Çalışma 2015-2016 eğitim-öğretim yılının güz döneminde uygulanmıştır. Çalışmaya Muğla ili Menteşe ilçe merkezindeki bir ortaokulda 5. sınıf düzeyinde öğrenim gören 27'si (14 Kız-13 Erkek) deney, 27'si (15 Kız-12 Erkek) kontrol grubunda olmak üzere toplam 54 öğrenci katılmıştır. Çalışmanın verileri Akademik Başarı Testi ve Fen Öğrenimine Yönelik Motivasyon Ölçeği ile toplanmıştır. Veriler Bağımlı t-testi, Bağımsız t-testi, Wilcoxon İşaretli-Sıralar testi ve Mann-Whitney U testi ile analiz edilmiştir. Fosil ve biyoçeşitlilik konularının öğretiminde hem müze rehberi hazırlama yoluyla öğretimin hem de çalışma yaprakları yoluyla öğretimin olumlu ve kalıcı etkileri olduğu tespit edilmiştir. Her iki öğretimin de öğrencilerin fen öğrenimine yönelik motivasyonları üzerinde olumlu etkileri olmadığı belirlenmiştir. Doğa tarihi müzelerinden fen öğrenmede müze rehberi hazırlama ve çalışma yaprakları yoluyla öğretimin kullanılması önerilmiştir.
-Anahtar kelimeler: fosil ve biyoçeşitlilik, doğa tarihi müzesi, müze çalışma yaprakları, müze rehberi hazırlama, fen öğrenimine yönelik motivasyon
+	 Biyoçeşitlilik su ve kara ortamlarındaki genetik, tür ve ekosistem çeşitliğidir. Son yıllarda insan kaynaklı faaliyetler sonucunda dünya genelinde biyoçeşitlilik de hızlı bir azalma mevcuttur. Dolayısıyla bireylerin bu azalma ile ilgili farkındalıklarını, düşüncelerini ve tutumlarını incelemek, yine insan kaynaklı çözüm önerileri geliştirmek adına önemlidir. Bu çalışmada ilköğretim (7. ve 8. sınıflar) ve lise (9. ve 10. Sınıflar) öğrencilerin biyoçeşitliliğin azalması ile ilgili görüşleri incelenmiştir. Yarı yapılandırılmış görüşmeler ve ilgili literatürden yararlanarak geliştirilen `Biyoçeşitliliğin Azalması ile İlgili Tutum ve Düşünceler' (BATD) ölçeği veri toplama aracı olarak kullanılmıştır. Kasıtlı örnekleme ile Ankara ilinden 290 ve Kırşehir ilinden 422 olmak üzere toplam 712 öğrenci çalışmaya katılmıştır. Verilerin analizinde yüzde ve ortalama gibi betimsel istatistikler ile açıklayıcı ve onaylayıcı faktör analizi, Mann-Whitney U testi gibi çıkarımsal istatistikler kullanılmıştır. Çalışma sonunda ilköğretim ve lise öğrencilerinin biyoçeşitliliğin azalması ile ilgili endişelerinin yüksek olduğu gözlenmiştir. Kızlar erkeklere göre daha endişeli iken, erkeklerin biyoçeşitliliğin azalmasını önlemede teknolojik çözümlere daha sıcak baktığı tespit edilmiştir. Ayrıca şehir (endüstrileşmiş ve endüstrileşmemiş) faktörünün tutumlarda etkili olmadığı sonucuna varılmıştır. Öğrenciler biyoçeşitliliğin azalmasının nedenleri olarak küresel ısınma ve asit yağmurları gibi küresel sorunları göstermiştir. Biyoçeşitliliğin azalmasının sonuçları için ise besin zincirinin bozulması ve doğal dengenin bozulması ön plana çıkmıştır. Biyoçeşitliliğin azalmasını önleme yöntemleri ile ilgili olarak öğrenciler geri dönüşüm ve ağaçlandırmaların etkili olacağını düşünmüştür.Anahtar kelimeler: Biyoçeşitlilik, biyoçeşitliliğin azalması, çevre eğitimi, öğrenciler, düşünce, tutum
 	 </v>
       </c>
       <c r="I17" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	  Out of school learning environments that are suitable for non-formal learning include museums, science centers, zoos, parks, planetarium, etc. Museums are one of the out of school learning environments that are frequently visited for science education. Natural history museums are particularly appropriate for science education. Museum worksheets are one of the prevalently applied teaching strategies for science education in museums. There are still disagreements on the effectiveness of museum worksheets. New teaching strategies in museums are needed to be designed, implemented and evaluated. The aim of this study is to compare museum guide preparation and teachings with museum worksheets in natural history museum and their effects on students' science success on fossils and bio-diversity subjects and their motivations on science learning; and is to assess these effects permanence. Quasi-experimental method with nonequivalent control group modal was applied in the study. The study was conducted in fall term of 2015-2016 academic year. 5th grade 54 students including 27 (14 females-13 males) experiment group, and 27 (15 females-12 males) control group students studying in middle school in Menteşe town of Muğla. The data were obtained through Academic Success Test, and Students' Motivation Towards Science Learning Questionnaire. The data were analyzed through Dependent t-test, Independent t-test, Wilcoxon Signed-Rank test, and Mann-Whitney U test. It was identified that both museum guide preparation and museum worksheet teachings for fossils and biodiversities subjects were positive and had permanent effects. It was determined that the both teachings did not have positive effects on students' motivation towards science learning. It has been suggested to prefer a teaching strategy thorugh applying museum guide preparation and museum worksheets in science learning from natural history museums.
-Keywords: fossil and biodiversity, natural history museum, museum worksheets,museum guide preparation, motivation towards science learning</v>
+	  Biodiversity is the diversity of genetical sources, species and ecosystems in water and land environments. There is a fast biodiversity loss due to the anthropocentric activities in last decades. Therefore, it is crucial to understand individuals? awareness, ideas and attitudes about biodiversity loss in order to develop solutions. In the present study, primary and secondary school students? ideas and attitudes towards biodiversity loss were investigated. `Ideas and Attitudes towards Biodiversity Loss? scale, which was developed using semi-structured interviews and the scales in existing literature, was utilized as data collection tool. 290 students in Ankara and 422 students in Kırşehir (totally 712 students) constituted the purposeful sample. In data analysis, it was used descriptive statistics such as percentage and mean and inferential statistics such as explaratory and confirmatory factor analysis and Mann-Whitney U tests. The study showed that students possessed high level of concerns regarding biodiversity loss (BL). The girls were more anxious about BL than boys, whereas more boyes than girls agreed that technological solutions would resolve the problems about BL. In addition, the city factor (industrialized-nonindustrialized) did not exert influence on students? attitudes. Students presented global warming and acid raining as main reasons of BL. The collapses in food chaing and natural balance were the main results of BL. They also considered that recyling and planting trees would strop BL.Keywords: Biodiversity, biodiversity loss, environmental education, students, idea, attitude.</v>
       </c>
     </row>
     <row r="18" xml:space="preserve">
@@ -1043,12 +1015,20 @@
       </c>
       <c r="H18" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	 Biyoçeşitlilik su ve kara ortamlarındaki genetik, tür ve ekosistem çeşitliğidir. Son yıllarda insan kaynaklı faaliyetler sonucunda dünya genelinde biyoçeşitlilik de hızlı bir azalma mevcuttur. Dolayısıyla bireylerin bu azalma ile ilgili farkındalıklarını, düşüncelerini ve tutumlarını incelemek, yine insan kaynaklı çözüm önerileri geliştirmek adına önemlidir. Bu çalışmada ilköğretim (7. ve 8. sınıflar) ve lise (9. ve 10. Sınıflar) öğrencilerin biyoçeşitliliğin azalması ile ilgili görüşleri incelenmiştir. Yarı yapılandırılmış görüşmeler ve ilgili literatürden yararlanarak geliştirilen `Biyoçeşitliliğin Azalması ile İlgili Tutum ve Düşünceler' (BATD) ölçeği veri toplama aracı olarak kullanılmıştır. Kasıtlı örnekleme ile Ankara ilinden 290 ve Kırşehir ilinden 422 olmak üzere toplam 712 öğrenci çalışmaya katılmıştır. Verilerin analizinde yüzde ve ortalama gibi betimsel istatistikler ile açıklayıcı ve onaylayıcı faktör analizi, Mann-Whitney U testi gibi çıkarımsal istatistikler kullanılmıştır. Çalışma sonunda ilköğretim ve lise öğrencilerinin biyoçeşitliliğin azalması ile ilgili endişelerinin yüksek olduğu gözlenmiştir. Kızlar erkeklere göre daha endişeli iken, erkeklerin biyoçeşitliliğin azalmasını önlemede teknolojik çözümlere daha sıcak baktığı tespit edilmiştir. Ayrıca şehir (endüstrileşmiş ve endüstrileşmemiş) faktörünün tutumlarda etkili olmadığı sonucuna varılmıştır. Öğrenciler biyoçeşitliliğin azalmasının nedenleri olarak küresel ısınma ve asit yağmurları gibi küresel sorunları göstermiştir. Biyoçeşitliliğin azalmasının sonuçları için ise besin zincirinin bozulması ve doğal dengenin bozulması ön plana çıkmıştır. Biyoçeşitliliğin azalmasını önleme yöntemleri ile ilgili olarak öğrenciler geri dönüşüm ve ağaçlandırmaların etkili olacağını düşünmüştür.Anahtar kelimeler: Biyoçeşitlilik, biyoçeşitliliğin azalması, çevre eğitimi, öğrenciler, düşünce, tutum
+	 Bu araştırmanın amacı, ortaokul öğrencilerinin (5,6,7, ve 8.Sınıf), Biyolojik çeşitlilik konusundaki bilişsel yapılarını ortaya koymak, kavramsal anlam düzeylerindeki değişim sürecini sınıf düzeylerine göre tespit etmektir. Bu çalışma nitel bir araştırma olup, araştırmada betimsel araştırma yöntemleri içerisinde yer alan ve nitel araştırma desenlerinden gelişimsel araştırma deseni kullanılmıştır.
+Araştırmanın örneklemini, 2017-2018 eğitim-öğretim yılı, bahar döneminde, Bursa ilinde öğrenim gören 5, 6, 7 ve 8. Sınıflardan oluşan toplam 308 ortaokul öğrencisi oluşturmaktadır. Veri toplama aracı olarak kelime ilişkilendirme testlerinden yararlanılmıştır. Kelime ilişkilendirme testlerinde "ekosistem, biyolojik çeşitlilik, besin zinciri, tür, nesli tükenmekte olan canlılar, çevre sorunları ve çevre koruma" olmak üzere yedi anahtar kavram kullanılmıştır. Verilerin analiz sürecinde, frekans tablosu kullanılarak kesme noktası tekniği ile kavram ağları oluşturulmuş ve ilgili kavramlara yönelik ortaokul öğrencilerinin bilişsel yapılarının karşılaştırması sağlanmıştır. Kavram ağlarından elde edilen sonuçlara göre bulgular yorumlanmıştır. Sonuç olarak, ortaokul öğrencilerinin (5,6,7 ve 8. Sınıf), nesli tükenmekte olan canlılar, çevre sorunları ve çevre koruma anahtar kavramlarını doğru ilişkilendirdiği sonucuna varılmıştır. Ayrıca, besin zinciri, tür ve ekosistem anahtar kavramını 8.sınıf öğrencilerinin genel olarak doğru ilişkilendirdiği, biyolojik çeşitlilik anahtar kavramını genel olarak 5.sınıf öğrencilerinin doğru ilişkilendirdiği, 6. ve 7.sınıf öğrencileri tarafından besin zinciri, tür, biyolojik çeşitlilik ve ekosistem anahtar kavramlarının tam olarak anlaşılamadığı sonucuna varılmıştır.
+Kelime ilişkilendirme testinde ortaokul öğrencilerinin en fazla ilişkilendirdiği anahtar kavramlar nesli tükenmekte olan canlılar, çevre sorunları ve çevre korumadır. En az ilişkilendirilen anahtar kavramlar, besin zinciri, tür, biyolojik çeşitlilik ve ekosistemdir. Hayvan, bitki, insan, meyve, yiyecek/besin, çevre kirliliği, su kirliliği, kirlilik, küresel ısınma, çöp, filtre, ağaç ve temizlik kavramları öğrencilerin en fazla kullandığı kavramlardır.  
+Veri toplam aracı olarak kullanılan kelime ilişkilendirme testinde öğrencilerin her bir anahtar kavramla ilgili cümle kurmaları da istenmiştir. Bu cümleler içerdiği bilgi ve anlam açısından incelenip sınıflandırılarak cümlelerin analizi gerçekleştirilmiştir. Elde edilen sonuçlara göre ortaokul öğrencilerinin (5,6,7 ve 8.sınıf) en fazla sayıda nesli tükenmekte olan canlılar, çevre sorunları ve çevre koruma anahtar kavramları ile ilgili anlamlı cümleler kurdukları ortaya çıkmıştır. 
+Araştırmada, eğitim-öğretim sonucunda, kazanılan bilgi, deneyim ve farkındalık arttıkça, televizyon, basın, internet gibi ortamlardan edindikleri bilgiler ile öğrencilerin bilimsel bilgiye daha yakın cevaplar verdikleri tespit edilmiştir. Aynı zamanda fen bilimleri öğretim programında biyoçeşitlilik kavramına ilişkin kazanım sayısı arttıkça öğrencilerin bilgi ve beceri seviyesinin daha yüksek olduğu sonucuna varılmıştır.
 	 </v>
       </c>
       <c r="I18" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	  Biodiversity is the diversity of genetical sources, species and ecosystems in water and land environments. There is a fast biodiversity loss due to the anthropocentric activities in last decades. Therefore, it is crucial to understand individuals? awareness, ideas and attitudes about biodiversity loss in order to develop solutions. In the present study, primary and secondary school students? ideas and attitudes towards biodiversity loss were investigated. `Ideas and Attitudes towards Biodiversity Loss? scale, which was developed using semi-structured interviews and the scales in existing literature, was utilized as data collection tool. 290 students in Ankara and 422 students in Kırşehir (totally 712 students) constituted the purposeful sample. In data analysis, it was used descriptive statistics such as percentage and mean and inferential statistics such as explaratory and confirmatory factor analysis and Mann-Whitney U tests. The study showed that students possessed high level of concerns regarding biodiversity loss (BL). The girls were more anxious about BL than boys, whereas more boyes than girls agreed that technological solutions would resolve the problems about BL. In addition, the city factor (industrialized-nonindustrialized) did not exert influence on students? attitudes. Students presented global warming and acid raining as main reasons of BL. The collapses in food chaing and natural balance were the main results of BL. They also considered that recyling and planting trees would strop BL.Keywords: Biodiversity, biodiversity loss, environmental education, students, idea, attitude.</v>
+	  The purpose of this research is to reveal the cognitive structures of middle school students (5th, 6th, 7th, and 8th grades) on biological diversity and to determine the process of change in their conceptual meaning levels by grade level. This is a qualitative research. It uses the developmental research design, which is a descriptive research method and a qualitative research design. 
+The research sample of consists of a total of 308 5th-, 6th-, 7th-, and 8th-grade middle school students studying in Turkey's Bursa province in the spring semester of the 2017-2018 academic year. Word association tests were used for data collection. Seven key concepts were used in the word association tests: "ecosystem, biological diversity, food chain, species, endangered creatures, environmental problems, environmental protection". In the data analysis process, concept networks were created by the cut-off point technique using the frequency table, thereby making a comparison of the middle school students' cognitive structures for the related concepts. Findings were interpreted based on the results obtained from the concept networks. As a result, it was found that the middle school students (5th, 6th, 7th, and 8th grades) correctly associated the key concepts of endangered creatures, environmental problems, and environmental protection. In addition, it was determined that the 8th grade students correctly associated the key concepts of food chain, species, and ecosystem in general, while the 5th grade students correctly associated the key concept of biological diversity in general, and that the 6th and 7th grade students could not fully understand the key concepts of food chain, species, biological diversity and ecosystem.
+The key concepts that the middle school students associated in the word association test most were endangered creatures, environmental problems, and environmental protection. The least associated key concepts were found to be food chain, species, biological diversity, and ecosystem. The concepts the students used most were animal, plant, human, fruit, food/nutrient, environmental pollution, water pollution, pollution, global warming, garbage, filter, tree, and cleanliness.  
+In the word association test used as a data collection tool, the students were also asked to make sentences about each key concept. Those sentences were examined and classified in terms of the information and meaning they contained, and the analysis of the sentences was performed. Based on the obtained results, it was revealed that the middle school students (5th, 6th, 7th, and 8th grades) made the biggest number of meaningful sentences about the key concepts of endangered creatures, environmental problems, and environmental protection. 
+The study concluded that as the knowledge, experience, and awareness gained through the educational process increased, the students gave answers closer to scientific knowledge, along with the information they obtained from media such as television, press, and the internet. Furthermore, it was concluded that as the number of learning outcomes related to the concept of biological diversity in the science curriculum increased, the students' levels of knowledge and skill rose as well.</v>
       </c>
     </row>
     <row r="19" xml:space="preserve">
@@ -1203,38 +1183,6 @@
       </c>
       <c r="H21" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	 Bu çalışmanın amacı, fen bilimleri öğretmenlerinin sosyobilimsel konulara (SBK) yönelik tercih ettikleri roller ve rolleri tercih etme/etmeme nedenlerinin, derslerinde kullanmış oldukları iletişimsel yaklaşım ve söylem desenleriyle ilişkilendirilmesi ve bu bağlamda SBK içeren ve SBK içermeyen konuların karşılaştırılmasıdır. Bu çalışma, nitel araştırma yaklaşımına uygun olarak bütüncül tekli durum deseniyle tasarlanmıştır. Çalışma grubunun oluşturulabilmesi için öncelikle kolay ulaşılabilir örnekleme ile Milli Eğitim Bakanlığı bünyesinde görev yapan 10 fen bilimleri öğretmenine ulaşılmıştır. Öğretmenler ile yapılan yarı yapılandırılmış görüşmeler sonucunda, derslerine sosyobilimsel konuları dâhil eden ve bunu derslerine nasıl taşıdığına yönelik örnekler verenler arasından dört fen bilimleri öğretmeni amaçlı olarak ölçüt (kriter) örneklem ile seçilmiştir. Seçilen bu dört öğretmene SBK'ya Yönelik Öğretmen Rolleri Vignetleri uygulanmıştır. Yapılan görüşmeler doğrultusunda öğretmenlerin ortak olarak 5. sınıf kademesinin fen derslerine girdikleri tespit edildikten sonra, araştırmacı tarafından seçilen biyoçeşitlilik ile ısı ve sıcaklık konularındaki dersleri video ve ses kaydına alınmıştır. Veri analizlerinde söylem analizi kullanılmıştır. Çalışmada veriler iletişimsel yaklaşım ve söylem desenlerine göre analiz edilmiştir. Video kayıtları analizleri, bu çalışmada geliştirilen barkod sistemi ile sunulmuştur. Araştırmanın sonunda, çalışmaya katılan öğretmenlerden üçünün nötr tarafsızlık rolünü seçtiği ve birinin ise kararlı tarafsızlık rolünü seçtiği görülmüştür. Öğretmenlerin ders video analizleri sonucunda, nötr tarafsızlık rolünü seçen öğretmenlerden biri ile kararlı tarafsızlık rolünü seçen öğretmenin derste özel nötrallik rolü sergilediği tespit edilmiştir. Yani çalışmadaki iki öğretmenin tercih ettiği rol ile derslerinde sergilediği rolün birbirinden farklı olduğu görülmüştür. Öğretmenlerin SBK içeren dersleri ile SBK içermeyen dersleri karşılaştırıldığında; nötr tarafsızlık rolünde olan iki öğretmenin de biyoçeşitlilik konusunda sıklıkla diyalojik yaklaşım ve açık zincir söylem desenini, ısı ve sıcaklık dersinde ise sıklıkla otoriter yaklaşım ve kapalı zincir söylem desenini kullandıkları tespit edilmiştir. Özel nötrallik rolünü sergileyen her iki öğretmenin de her iki konuda sıklıkla otoriter yaklaşım ile kapalı zincir ve üçlü söylem desenlerini kullandıkları görülmüştür. Bu doğrultuda SBK'larda nötr tarafsızlık rolünde olan öğretmenlerin diyalojik bir yaklaşım ile değerlendirmeci olmayan açık ve kompleks zincir söylem desenlerini kullandığı, özel nötrallik rolünde olan öğretmenlerin ise otoriter bir yaklaşım ve değerlendirmeci olan üçlü ve kapalı zincir söylem desenlerini kullandığı sonucuna ulaşılmıştır. Elde edilen bulgular doğrultusunda yeni çalışmalara ışık tutabilecek önerilerde bulunulmuştur.
-	 </v>
-      </c>
-      <c r="I21" t="str" xml:space="preserve">
-        <v xml:space="preserve"> 
-	  The aim of this study is to associate science teachers' their preferred roles and reasons for choosing this roles for socioscientific issues (SSI), with the communicative approach and discourse patterns they used in their courses, and to compare socioscientific issues and classical science subjects in this context. In this qualitative study, the holistic single case study design, one of the types of case studies, was used. In order to create a working group, 10 science teachers working within the Ministry of Education were reached with easily accessible sampling. As a result of the semi-structured interviews with these teachers four science teachers were selected with a criterion sample of including socioscientific issues in their courses and giving examples of how they carry this issues to their courses. These to four selected teachers implemented the Teacher's Roles in SSI Discourse. According to the interviews conducted, it was determined that teachers entered the same level science class of the fifth grade; then the lessons on biodiversity and heat and temperature subjects were recorded on video and audio by the researcher. Discourse analysis was used in data analysis. In the study, the data were analyzed as regards to communicative approaches and discourse patterns Analysis of video recordings was presented with a barcode system developed in this study. At the end of the study, it was observed that three of the teachers' involved in the study chose neutral impartiality role, and one teacher chose committed impartiality role. As a result of the teachers' course video analysis, one of the teachers who chose the role of neutral impartiality and one of the teacher who chose the role of committed impartiality were found to exhibit exclusive neutrality role in the lesson. In other words, it was seen that the role preferred by the two teachers in the study and the role they displayed in their lessons differed from each other. Comparing teachers' SSI lessons with classical science subject it was concluded that teachers in the role of neutral impartiality often use the dialogic approach and open chain discourse pattern in biodiversity, and in heat and temperature subject, they often use the authoritarian approach and closed chain discourse pattern. Exhibiting the role of exclusive neutrality, both teachers have often used closed chain and triple discourse patterns with authoritarian approach on both subjects. In this direction, it was concluded that teachers in the role of neutral impartiality in SSI use open and complex chain discourse patterns that are not evaluative with a dialogic approach, while teachers in the role of exclusive neutrality use triple and closed chain discourse patterns that are authoritarian approach and evaluative. According to the results obtained, suggestions have been made that may shed light on new studies.</v>
-      </c>
-    </row>
-    <row r="22" xml:space="preserve">
-      <c r="A22" t="str">
-        <v>48</v>
-      </c>
-      <c r="B22" t="str">
-        <v>538459</v>
-      </c>
-      <c r="C22" t="str">
-        <v>ZEYNEP ÖZYURT</v>
-      </c>
-      <c r="D22" t="str">
-        <v>2019</v>
-      </c>
-      <c r="E22" t="str">
-        <v>Fen bilgisi öğretmen adaylarının biyolojik çeşitlilik konusundaki farkındalık ve davranış düzeylerinin belirlenmesiDetermination of awareness and behavior levels of biological diversity of science teacher candidates</v>
-      </c>
-      <c r="F22" t="str">
-        <v>Yüksek Lisans</v>
-      </c>
-      <c r="G22" t="str">
-        <v>Eğitim ve Öğretim = Education and Training</v>
-      </c>
-      <c r="H22" t="str" xml:space="preserve">
-        <v xml:space="preserve"> 
 	 Bu araştırmanın amacı Argümantasyon Tabanlı Bilim Öğrenme (ATBÖ) yaklaşımın öğrencilerin akademik başarısına ve derse yönelik tutumlarının yanı sıra karar verme, argümantasyon, tartışma ve problem çözme becerilerine etkisini belirlemektir.
 Araştırmada statik grup karşılaştırmalı desen kullanılmıştır. Kontrol grubunu oluşturan 23 ve deney grubunu oluşturan 17 öğrenci olmak üzere 10. Sınıfta öğrenim gören toplam 40 öğrenci ile birlikte Muş'ta bulunan bir kız lisesinde gerçekleştirilmiştir. Kontrol grubunda bulunan öğrencilere "Kalıtım ve Biyoçeşitlilik" konusunda mevcut öğretim yöntemlerine ilişkin etkinlikler ve deney grubunda bulunan öğrencilere ise ATBÖ yaklaşımına ilişkin etkinlikler uygulanmıştır.
 Uygulamaların sonunda öğrencilere nicel veri toplama aracı olarak Biyoloji Soru Formu, Biyoloji Bilimine ve Dersine Yönelik Tutum Ölçeği (BBDTÖ), Karar Verme Becerilerini Değerlendirme Ölçeği, Argümantasyon Testi, Tartışmacı Anketi ve Problem Çözme Ölçeği kullanılmıştır. Veriler analiz programında Shapiro-Wilk ve ilişkisiz örneklemler t-testi kullanılarak analiz edilmiştir.
@@ -1242,6 +1190,43 @@
 Anahtar Kelimeler: Argüman, Argümantasyon, Argümantasyon Tabanlı Bilim Öğrenme, Karar Verme, Tartışma, Problem Çözme
 	 </v>
       </c>
+      <c r="I21" t="str" xml:space="preserve">
+        <v xml:space="preserve"> 
+	  The purpose of this study was to analyze the effects of Argument-Based Inquiry (ABI) approach (adopted from the Science Writing Heuristic-SWH approach) to students' academic success, their attitude towards classes, decision making skills, argumentation, discussion and, problem solving skills. Static-group comparison design was used in the research. 40 students who attended 10th grade in a girl high school in Muş participated in the research. 23 of them were the control group where as 17 of them were the experimental group. The control group was taught "Heredity and Bio-diversity" in the current teaching methods whereas the experimental group was taught the same subject with ABI approach. At the end of the application process students were given quantitatve data collecting tools such as: Biology Question Form, Biology Science and Course Attitude Scale, Decision-making ability Evaluation Scale, Argumentation Test, Argumentative Scale and Problem Solving Scale. Datas were analyzed with Shapiro-Wilk and unrelated samples T-test in analysis program. According to the results of the research, It was observed that Argument-based Inquiry Approach contributed to student's academic success, their attitude towards classes, decision making skills, argumentation, discussion and, problem solving skills.
+Keywords: Argument, Argumentation, Argument Based Inquiry Approach, Decision Making, Discussion, Problem Solving</v>
+      </c>
+    </row>
+    <row r="22" xml:space="preserve">
+      <c r="A22" t="str">
+        <v>48</v>
+      </c>
+      <c r="B22" t="str">
+        <v>538459</v>
+      </c>
+      <c r="C22" t="str">
+        <v>ZEYNEP ÖZYURT</v>
+      </c>
+      <c r="D22" t="str">
+        <v>2019</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Fen bilgisi öğretmen adaylarının biyolojik çeşitlilik konusundaki farkındalık ve davranış düzeylerinin belirlenmesiDetermination of awareness and behavior levels of biological diversity of science teacher candidates</v>
+      </c>
+      <c r="F22" t="str">
+        <v>Yüksek Lisans</v>
+      </c>
+      <c r="G22" t="str">
+        <v>Eğitim ve Öğretim = Education and Training</v>
+      </c>
+      <c r="H22" t="str" xml:space="preserve">
+        <v xml:space="preserve"> 
+	 Bu araştırmanın amacı Argümantasyon Tabanlı Bilim Öğrenme (ATBÖ) yaklaşımın öğrencilerin akademik başarısına ve derse yönelik tutumlarının yanı sıra karar verme, argümantasyon, tartışma ve problem çözme becerilerine etkisini belirlemektir.
+Araştırmada statik grup karşılaştırmalı desen kullanılmıştır. Kontrol grubunu oluşturan 23 ve deney grubunu oluşturan 17 öğrenci olmak üzere 10. Sınıfta öğrenim gören toplam 40 öğrenci ile birlikte Muş'ta bulunan bir kız lisesinde gerçekleştirilmiştir. Kontrol grubunda bulunan öğrencilere "Kalıtım ve Biyoçeşitlilik" konusunda mevcut öğretim yöntemlerine ilişkin etkinlikler ve deney grubunda bulunan öğrencilere ise ATBÖ yaklaşımına ilişkin etkinlikler uygulanmıştır.
+Uygulamaların sonunda öğrencilere nicel veri toplama aracı olarak Biyoloji Soru Formu, Biyoloji Bilimine ve Dersine Yönelik Tutum Ölçeği (BBDTÖ), Karar Verme Becerilerini Değerlendirme Ölçeği, Argümantasyon Testi, Tartışmacı Anketi ve Problem Çözme Ölçeği kullanılmıştır. Veriler analiz programında Shapiro-Wilk ve ilişkisiz örneklemler t-testi kullanılarak analiz edilmiştir.
+Araştırmanın sonuçlarına göre Argümantasyon Tabanlı Bilim Öğrenme Yaklaşımının öğrencilerin akademik başarılarına, biyoloji dersine yönelik tutumlarına, karar verme, argümantasyon, tartışma ve problem çözme becerilerine olumlu katkı sağladığı gözlenmiştir.
+Anahtar Kelimeler: Argüman, Argümantasyon, Argümantasyon Tabanlı Bilim Öğrenme, Karar Verme, Tartışma, Problem Çözme
+	 </v>
+      </c>
       <c r="I22" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
 	  The purpose of this study was to analyze the effects of Argument-Based Inquiry (ABI) approach (adopted from the Science Writing Heuristic-SWH approach) to students' academic success, their attitude towards classes, decision making skills, argumentation, discussion and, problem solving skills. Static-group comparison design was used in the research. 40 students who attended 10th grade in a girl high school in Muş participated in the research. 23 of them were the control group where as 17 of them were the experimental group. The control group was taught "Heredity and Bio-diversity" in the current teaching methods whereas the experimental group was taught the same subject with ABI approach. At the end of the application process students were given quantitatve data collecting tools such as: Biology Question Form, Biology Science and Course Attitude Scale, Decision-making ability Evaluation Scale, Argumentation Test, Argumentative Scale and Problem Solving Scale. Datas were analyzed with Shapiro-Wilk and unrelated samples T-test in analysis program. According to the results of the research, It was observed that Argument-based Inquiry Approach contributed to student's academic success, their attitude towards classes, decision making skills, argumentation, discussion and, problem solving skills.
@@ -1344,16 +1329,12 @@
       </c>
       <c r="H25" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	 İnsanın yeryüzündeki varoluşunun etkileri bugün anlam krizi, sosyal krizler, ekolojik kriz gibi çeşitli problemlerle birlikte anılmakta ve her bir kriz durumu insan hakkında yeniden düşünmeyi zorunlu kılmaktadır. Biyoçeşitlilikte azalma, artan çevre kirliliği, küresel ısınma, tatlı su kaynaklarının azalması, sel ve kuraklık gibi çeşitli sonuçları bulunan ekolojik kriz yalnızca insan varlığını değil gezegenin tüm yaşam formlarını etkilemesi sebebiyle alarmist bir tonla tartışmalara konu olmaktadır. 1960'larda başlayıp günümüze kadar devam eden bu tartışmalar etik ve felsefi birtakım teorilerin ortaya çıkışını hazırlamış ve ilgili teorilerin odağında ise, çevresel krizin temelinde antroposantrik dünya görüşünün bulunduğu iddiası yer almıştır. 
-Antroposantrik dünya görüşlerinin dayanaklarından biri olarak dinlere işaret edilmiş olması göz önüne alınarak, din eğitiminin insan tasavvurunun ne olduğu ve yüzleştiği/yüzleşeceği sorunlar karşısında 21. yüzyıl insanına ne sunduğu sorusu araştırmaya değer görülmüştür. Bu noktada tezin amacı; din eğitiminde insan tasavvurunun anlaşılmasına katkıda bulunmak için Din Kültürü ve Ahlak Bilgisi ders kitaplarında, insana dair açık ve örtük söylemlerin analiz edilmesi olarak belirlenmiştir. Eleştirel söylem analizinin yöntem olarak benimsendiği bu çalışma için 2018 yılında okutulmaya başlanan 4-12. sınıflara ait MEB yayınevi tarafından yayınlanmış 9 kitap analiz edilmiştir. 
-Çalışma öncelikle ders kitaplarında dini anlatıya başvurularak insanın ayrıcalıklı bir varlık olduğuna dair kabul ve tahayyüllerin öne çıkarıldığını göstermiştir. Bunu yaparken insanın üstün özelliklerle yaratılışının merkeze alındığı, yaşamın insan ihtiyaçları ve deneyimleri etrafında şekillendiği bir anlam dünyasının resmedildiği, ahlakın ve hukukun kapsamı konusunda insanlar arası ilişkilerin vurgulandığı görülmüştür. İnsanolmayanlara yönelik söylemlerin insan ilgi ve ihtiyaçları çerçevesinde anlatıya dahil edilmesi araçsallaştırıcı bir tavır olarak değerlendirilmiştir. Antroposantrik dünya görüşüne konu edilen söylemlerle paralellik gösteren bu tespitler neticesinde ders kitaplarının yaşadığımız çağın en acil sorunu olarak görünen ekolojik krizle ilgili anlamlı bir çözüm üretecek düşünce, tutum ve davranış sunmaktan uzak olduğu sonucuna ulaşılmıştır.
+	 Bu çalışmada öğretmenlerin küresel olarak gördükleri ve en çok önemsedikleri çevre sorununun ne olduğu, bu sorun veya diğer çevre sorunlarına yönelik hayatlarında neler yaptıkları, ne kadar sürdürülebilir yaşama dikkat ettikleri üzerinde durulmuştur. Bunun yanı sıra öğretmenlerin kendi bilgilerini ve hayat deneyimlerini çocuklara yansıtması, onların çevre eğitimine ne şekilde katkıda bulunduklarına ve kendilerini bu konuda yeterli görüp görmediklerine dair öz değerlendirmelerini de incelemek amaçlanmaktadır. Araştırmada nitel araştırma yöntemlerinden olgu bilim deseni kullanılmış ve çalışma grubu belirlenirken amaçlı örnekleme yöntemlerinden kartopu örnekleme yöntemi tercih edilmiştir. Araştırmanın çalışma grubunu Artvin iline bağlı Borçka ve Hopa ilçesinde görev yapan 20 okul öncesi öğretmeni oluşturmaktadır. Araştırmada temel veri toplama yöntemi olarak görüşme kullanılmıştır. Araştırmada görüşmelerden elde edilen nitel verilerin analizinde betimsel analiz tekniği kullanılmıştır. Verilerin analizi sonucunda öğretmenlerin çevre sorunlarının farkında olduğu ve su kirliliği, atık kirliliği, geri dönüşüm, plastikler, hava kirliliği ve tüketim alışkanlıkları üzerinde durdukları görülmüştür. Öğretmenlerin "çevresel sürdürülebilirlik" kavramına uzak oldukları, konunun su, atık, enerji yönetimi ve biyoçeşitlilik şeklinde detaylandırılıp desteklenerek sürdürülebilirlik kavramını ifade edebildikleri görülmüştür. Öğretmenlerin farkında olmadan sürdürülebilir adımlar attıkları da görülmüştür. Ayrıca görüşme yapılan katılımcıların pek çoğunun çevre eğitimi almamış olması ve alınabilecek eğitimlere nitelik açısından sıcak bakmıyor oluşları da doğru çevre eğitiminin öğretmen yeterliliklerini artırması açısından önemini ortaya koymaktadır.
 	 </v>
       </c>
       <c r="I25" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	  The effects of human existence on earth are mentioned together with various problems such as meaning crisis, social crisis, ecological crisis etc. and each crisis necessitates rethinking about human. The ecological crisis, which has various consequences such as decrease in biodiversity, increasing environmental pollution, global warming, decrease in freshwater resources, flood, and drought is the subject of discussions with an alarming tone because it affects not only human existence but also all life forms of the planet. These debates, which started in the 1960s and continued until today, have prepared the emergence of some ethical and philosophical theories, and the focus of the relevant theories has been the claim that the anthropocentric worldview is at the root of the environmental crisis.
-Considering the fact that religions are pointed out as one of the pillars of anthropocentric worldviews, the question of what religious education's image of human and what it offers to 21st century people in the face of the problems they face/will face has been deemed worthy of research. At this point, the aim of the thesis; In order to contribute to the understanding of image of human in religious education, it has been determined as the analysis of explicit and implicit discourses about human beings in Religious Culture and Moral Knowledge textbooks. For this study discourse analysis was adopted as a method and 9 textbooks, which are published by Ministry of Education, from grade 4th to 12th were analyzed.
-The study firstly showed that the acceptances and image of human being as a privileged being were emphasized by referring to the religious narrative in the textbooks. While doing this, it has been seen that the creation of human beings with superior characteristics is centered, a world of meaning in which life is shaped around human needs and experiences is depicted, and interpersonal relations are emphasized in the scope of morality and law. The inclusion of discourses about nonhumans in the narrative within the framework of human interests and needs has been evaluated as an instrumentalizing attitude. As a result of these findings, which are in parallel with the discourses on anthropocentric worldview, it has been concluded that the textbooks are far from presenting thoughts, attitudes and behaviors that will produce a meaningful solution to the ecological crisis, which seems to be the most urgent problem of our age.</v>
+	  In this study, it is emphasized that the most significant and global problem which is teachers' consider and, what are they doing in their lives about the other environmental problems, and, to what degree are they paying attention to sustainable life. Besides, it is aimed to examined self evaluation which is about teachers' reflection of their own knowledge and life experiments to students and their contribution to environment education and whether they consider themselves sufficient or not. In this research, phenomenology pattern which is one of the qualitative research method was used. When study group was determined, snowball examplication that is one of the intentional examplication methods was preffered. The study groups of the research are 20 pre-school departments working in Borçka and Hopa departments of Artvin. It is used as a basic data collection method in research and to prepare for pre-school education. Content analysis technique was used in the analysis of the qualitative data obtained from the interviews. As a result of the analysis of the data, it was seen that the teachers were aware of environmental problems and focused on water pollution, waste pollution, recycling, plastics, air pollution and consumption habits. It has been observed that the teachers are far from the concept of "environmental sustainability" and that they can express the concept of sustainability by detailing and supporting the subject as water, waste, energy management and biodiversity. It has been observed that teachers take sustainable steps without realizing it. Also, in terms of classroom education, it shows environmental education incompletely. In addition, the fact that most of the interviewed participants did not receive environmental education and that they do not look at the trainings that can be received in terms of quality reveals the importance of the right environmental education in terms of increasing teacher competencies.</v>
       </c>
     </row>
     <row r="26" xml:space="preserve">
@@ -1490,19 +1471,14 @@
       </c>
       <c r="H29" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	 Dünyada varlığı bilinen ve kabul edilen 8 deniz kaplumbağa türü bulunmaktadır. Bu deniz kaplumbağası türlerinden Caretta caretta ve Chelonia mydas ülkemiz denizini ve kıyılarını yuvalama ve yaşam alanı olarak seçmektedir. Ancak dünyada ve ülkemizde bulunan bu canlıların yaşam alanları turizm,bilinçsiz yapılaşma, yasa dışı  avlanma , çevre kirliliği ve en önemlisi de  insanların bu canlılaR hakkında yeteri kadar bilgi sahibi olmaması nedeniyle tahrip olmakta, bu hayvanların  nesli tehdit altına girmekte ve hatta tükenmektedir.
-Son yıllarda Çanakkale kıyılarında Caretta caretta ve Chelonia mydas deniz kamplumbağası türlerine beslenme ve üreme dönemlerindeki göçler, av araçları ile etkilişimleri ve küresel ısınmaya bağlı olarak giderek artan iklim değişiklikleri nedeniyle daha sık rastlanıldığı söylenebilir. Ancak bunun yanı sıra Çanakkale kıyılarına ölü ya da yaralı olarak  kıyıya vuran deniz kaplumbağalarının Çanakkale Onsekiz Mart Üniversitesi Deniz Kaplumbağaları Araştırma ve Uygulama Merkezi (ÇOMU DEKUM)'ne yapılan ihbarlar neticesinde Çanakkale denizi kıyılarının deniz kaplumbağalarının habitatı olabileceğini düşündürmektedir.
-İnsanlar ekolojik bir sistemi ve onunla olan bağlantılarını anladıklarında, ekosistemi bozma ihtimalleri daha düşük  olmaktadır. Ekolojik bilginin oluşturulmasında koruma ve farkındalık eğitim programları geliştirilerek daha sağlıklı sürdürülebilir ekosistemler oluşturulabilmek mümkündür. Çocuklar sınıf ortamında yaşadıkları çevre hakkında daha fazla bilgi edindikçe, koruma çalışmalarına katılım gösterdikçe, yaşadıkları ekosisteme daha çok değer verir ve korunmasında özen gösterirler. Tüm bunların ışığında bu tez çalışmasında; Çanakkale ilinde deniz kaplumbağalarının korunmasına yönelik  farkındalık oluşturmak amacıyla, çocuklara verilecek planlı eğitim etkinliklerinin  hem  deniz kaplumbağalarının korunmasında hem de öğrencilerin çevreye karşı tutumlarına önemli ölçüde katkı sağlayacağı  ve etkili olacağı düşünülmüştür.
-Bu çalışma 2016-217 eğitim-öğretim yılında, Marmara bölgesinde  bulunan bir ilköğretim okulunda  öğrenim gören 5.sınıf öğrencilerinin deniz kaplumbağaları konusunda gerçekleştirilen etkinlikler ile farkındalıklarının arttırılması, bilgi düzeyinin belirlenmesi ve çevreye yönelik tutumlarının geliştirilmesi amaçlanmıştır. Araştırma nicel araştırma modeli olan ön test - son test kontrol gruplu desen (ÖSKD) çalışması olarak desenlenmiştir. ÖSKD'de gruplardan biri deney diğeri kontrol grubudur. Araştırmanın çalışma grubunu 80'i kontrol grubunda, 55'i deneysel grupta bulunan toplamda 135 öğrenci oluşturmaktadır. Kontrol grubunda mevcut öğretim yöntemi ile ders  işlenirken , deney grubuna ise aynı konu deniz kaplumbağalarına yönelik hazırlanan  eğitim etkinlikleri  kullanılarak araştırmacı rehberliğinde gerçekleştirilmiştir.  Araştırmada veri toplama aracı olarak çevre tutum ölçeği, çalışma kapsamında geliştirilen deniz kaplumbağaları farkındalık ölçeği ve deniz kaplumbağaları bilgi  testi kullanılmıştır. Ayrıca verilen eğitiminin kalıcılığını tespit etmek için ise takip çalışması yapılmıştır.
-Araştırmada uygulanan ölçeklerden elde edilen veriler SPSS 20.0 paket programında bağımlı ve bağımsız örneklem t-testi kullanılarak analiz edilmiştir. Analizler sonucunda; deniz kaplumbağalarıyla ilgili geliştirilen etkinlik uygulamalarının, ilköğretim 5.sınıf         öğrencilerinin deniz kaplumbağalarıyla ilgili bilgi düzeylerinde, çevre tutumlarında ve deniz kaplumbağalarının korunmasına yönelik farkındalıklarında deney grubu lehine  istatistiksel olarak anlamlı bir artış olduğu  tespit edilmiştir.
+	 Bu araştırma, eko okullarda çevre eğitimine yönelik kullanılan çocuk kitaplarının çevre eğitimi ögelerini içerip içermediğini belirlemek amacıyla yapılmıştır. Bu bağlamda araştırmacı tarafından 11 alt başlıktan ve 59 maddeden oluşan "Eko-okul Temalarına Göre Kitap İnceleme Formu" hazırlanmıştır. Araştırma, nitel araştırma kapsamında doküman analizi yöntemiyle yapılmış olup kitaplar hazırlanan kitap inceleme formuna göre incelenmiştir. Araştırmanın çalışma grubunu Aydın ili Milli Eğitim Müdürlüğüne bağlı beş farklı eko-okulda, öğretmenlerin çevre eğitimi uygulamalarında kullandıkları 40'ar çocuk kitabı amaçlı örnekleme yöntemiyle seçilmiş, toplam 200 kitaptan oluşan bir çalışma grubu oluşturulmuştur. Eko- okul Temalarına Göre Kitap İnceleme Formuna göre incelenen kitaplardan hiçbir alt başlığı içermeyen kitaplar araştırmadan çıkarılmış, kalan 118 kitap çalışmaya dâhil edilmiştir. Kitapların eko-okul temalarını hangi oranda içerdiğini belirlemek için frekans analizleri yapılmıştır.
+Araştırma sonucunda incelenen çocuk kitaplarının sırasıyla biyoçeşitlilik ve doğa, enerji, çöp, su ve atıklar ile ilgili olduğu görülmüştür. İklim değişikliği alt başlıklarına hiçbir kitapta rastlanmamış olup, evrensel vatandaşlık, gıda, sağlık ve refah, ulaşım, deniz ve sahil ile ilgili konuların çok az kitapta ele alındığı saptanmıştır.
 	 </v>
       </c>
       <c r="I29" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	  There are 8 known sea turtle species in the world. These sea turtle species, Caretta caretta and Chelonia, choose our country's sea and coast as a nesting and living area. However, the living spaces of these creatures in the world and in our country are being destroyed due to tourism, unconscious structuring, illegal hunting, environmental pollution and most importantly because of the insufficient knowledge of these creatures, and these animals are endangered and even endangered. In recent years, it can be said that Caretta caretta and Chelonia mydas sea turtle species are more common on the coasts of Çanakkale due to migrations during feeding and reproduction periods, their interaction with game equipment and increasing climate changes due to global warming. However, the sea turtles that come ashores of the Dardanelles as dead or injured, suggest that the coasts of the Dardanelles can be the habitat of the sea turtles as a result of the warnings made to the       Çanakkale Onsekiz Mart University Marine Turtles Research and Application Center (ÇOMU DEKUM).
-When people understand an ecological system and its connections to it, they are less likely to disrupt the ecosystem. It is possible to develop healthier sustainable ecosystems by developing conservation and awareness training programs in the creation of ecological information. The more children learn about the environment in which they live, the more they participate in conservation efforts, the more they value ecosystem and care for the protection of society.
-In the light of all these, in this study it is thought that a planned training program to be provided to children will contribute significantly to the protection of sea turtles and to the students' attitudes towards the environment in order to raise awareness of the protection of sea turtles in the province of Çanakkale. The aim of this study was to increase the awareness of the 5th grade students attending a primary school in the Maramara region in 2016-2017 academic year with the activities carried out on sea turtles, to determine their knowledge level and to improve their attitudes towards the environment. The research was designed as a pre -test and post - test control group design study which is a quantitative research model. One of the groups was the experimental group and the other was the control group. The study group consisted of 135 students, 80 in the control group and 55 in the experimental group. In the control group, the subject was taught with the current teaching method, and in the experimental group, the same subject was instructed under the guidance of the researcher using educational activities prepared for the sea turtles. Environmental attitude scale, sea turtle awareness scale and sea turtle knowledge test developed within the scope of the study were used as data collection instruments. In addition, a follow-up study was conducted to determine the permanence of the training given. 
-The data obtained from the scales applied in the study were analyzed by using independent and independent samples t-test in SPSS 20.0 package program. As a result of analysis; it has been determined that the activity applications developed for the the sea turtles have a statistically significant increase in the level of knowledge of the 5th grade students  about the sea turtles, their environmental attitudes and their awareness about the protection of sea turtles compeared to the experimental group</v>
+	  This specific research is constituted to check the existence of environmental factors in children books which are used in environmental education. Thus, "Book Review Form In Regard to Eco-School Themes", which are comprised of 11 sub-title and 59 subjects, has been prepared. Research was done by document analysis method which is included in Qualitative research. Also these books have been analyzed according to the control list. Study group of this research has been determined by sampling technique with a total of 200 books that are 40 books from each 5 different eco-school which are affiliated to the ministry of education in the city of Aydın. The books, which do not have any under title of book review form in regard to Eco-school themes, have been removed and finally, 118 books have remained. Frequency analysis has been done to determine in which ratio that books comprise eco-school themes.      
+The researches showed that children books are related to subjects about nature, energy, biodiversity, water, rubbish, and wastes respectively. While sub-topic of climate change has not occurred in any books, subjects of global citizenship, food, wealth and health, transportation, sea, and seaside have been approached in very few books.</v>
       </c>
     </row>
     <row r="30" xml:space="preserve">
@@ -1563,12 +1539,16 @@
       </c>
       <c r="H31" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	 Bu araştırmada, 10. sınıf biyoloji dersi kalıtım konusuyla ilgili karekod destekli eğitim materyalinin tasarlanması amaçlanmıştır. İki aşamada gerçekleştirilen çalışmada, nicel araştırma yöntemlerinden tasarım ve geliştirme araştırması kullanılmıştır. İlk aşamada; araştırmanın konusunun belirlenebilmesi amacıyla, toplam 506 lise öğrencisi ve öğretmen adayına Biyoloji Kavram Zorluk Anketi uygulanmıştır. Bu anket, Bursa ilinde 9-12. sınıfta öğrenim gören 398 lise öğrencisi ile Balıkesir Üniversitesi Necatibey Eğitim Fakültesinde birinci sınıfta öğrenim gören 108 öğretmen adayına uygulanmıştır. Sonuç olarak; 10. sınıf biyoloji konularından 'Kalıtım ve Biyoçeşitlilik' ünitesinin 'Kalıtım' bölümü araştırma konusu olarak tespit edilmiştir. İkinci aşamada, kalıtım konusunun neden zor olduğunu tespit edebilmek amacıyla, Balıkesir ilinde öğrenim gören 10. sınıf 414 lise öğrencisine ve ortaöğretimde görev yapan 22 biyoloji öğretmenine Kalıtım Zorluklar Anketi uygulanmıştır. Sonuç olarak; öğrenciler, konunun ayrıntılı olduğunu belirtirken, öğretmenler de kalıtımla ilgili kavramların birbirine karışmasını, konunun zorluk sebebi olarak belirtmişlerdir. Bu öğrenme güçlüklerin giderilmesi için öğrenciler, kalıtım konusuyla ilgili bilgilerin azaltılmasını; öğretmenler de kalıtım konusuyla ilgili videoların karekodlar halinde biyoloji kitaplarına konmasını önermişlerdir. Aynı aşamada, 22 biyoloji öğretmenine 10. sınıf biyoloji dersi kitabında anlatılan kalıtım konusunun öğretmenler tarafından genel bir değerlendirmesi için Ders Kitabı Anketi uygulanmıştır. Sonuç olarak, bilimsel içeriğin öğrenci düzeyinin üstünde olduğu ve görsellerin yetersiz kaldığı bulunmuştur. Aynı anket sonucunda, biyoloji öğretmenleri sorunların giderilmesi için öneri olarak; daha çok görsel materyallerin yeterli sayıda verilmesi ve bilimsel içeriğin öğrenci düzeyinde olması gerektiğini belirtmişlerdir. Aşamanın sonunda, tüm değerlendirmeler doğrultusunda, kalıtım konusunun öğrenmedeki zorluğunu gidermek adına, ders kitabında kullanılmak üzere ya da derste etkinlik kağıdı olarak verilmesi adına karekodlu eğitim materyali tasarlanmıştır.
+	 Biyolojik çeşitlilik, bir ülkenin hem ekonomik hem de kültürel zenginliği demektir. Fakat bilinçsiz davranışlar sonucu çevremiz ve biyolojik çeşitlilik tehdit altındadır. Bu tehdidin gün geçtikçe arttığı düşünüldüğünde, öğrencilerin bu konudaki farkındalığı ve eğitilmesi son derece önemlidir. Gelecek nesillere yaşanabilir bir dünya bırakabilmek, çevre okuryazarlığı gelişmiş, bilinçli ve duyarlı bireyler ile mümkün olacaktır. Bu çalışmada, lise öğrencilerine uygulanacak biyolojik çeşitlilik konulu proje tabanlı eğitimin öğrencilerde biyoloji dersi tutumuna ne derece etki ettiğinin araştırılması amaçlanmıştır. Araştırma Tokat Reşadiye de bir devlet lisesinde okuyan 40 öğrenci ile yürütülmüştür. Çalışmada, lise 10. sınıf öğrencilerinin biyoloji dersi tutumlarına yönelik tek grup öntest-sontest uygulamalı zayıf deneysel desen kullanılmıştır. Biyolojik çeşitlilik konu içerikli hazırlanan öğretim programı proje tabanlı öğretim yöntemi kullanılarak gerçekleştirilmiştir. Öğrencilere çevrelerindeki biyolojik çeşitliliği tehdit eden etmenler
+vii
+ile ilgili proje önerileri verilmiştir. Her bir öğrenci hazırladığı projeyi diğer arkadaşlarına sunmuş, böylece biyolojik çeşitlilik ve biyolojik çeşitliliği tehdit eden etmenler derinlemesine incelenmiştir. Verilerin toplanmasında Tosun (2011) tarafından geliştirilen "Biyoloji dersi tutum ölçeği" kullanılmıştır. Uygulanan ölçek sorularından öntest ve sontestte elde edilen veriler, betimsel istatistikler ve Wilcoxon İşaretli Sıralar Testi ile değerlendirilmiştir. Araştırma sonucunda, öğrencilerin biyolojiye karşı tutumlarına ilişkin öntest-sontest puanları arasında sontest lehine anlamlı bir farklılık olduğu (anlamlılık değeri 0,003 (Z) -2,974) tespit edilmiştir. Uygulanan proje tabanlı eğitimin öğrencilerin akademik başarı değişkenine göre birinci ve ikinci sınav puanları arasında anlamlı bir fark olduğu (anlamlılık değeri 0,000 (Z) -5,277) saptanmıştır. Öğrencilerin biyoloji dersi tutumlarına ilişkin cinsiyet değişkenine göre öntest-sontest puanları arasında da anlamlı bir farklılık olduğu (kız öğrenciler için anlamlılık değeri 0,019 (Z) -2,336; erkek öğrenciler için anlamlılık değeri 0,064 (Z) -1,853 belirlenmiştir. Çalışma sonuçlara göre; öğrencilere uygulanan biyolojik çeşitlilik konulu proje tabanlı eğitimin, öğrencilerin biyoloji dersine olan tutumlarını ve biyoloji dersi akademik başarılarını olumlu yönde etkilediği anlaşılmıştır.
 	 </v>
       </c>
       <c r="I31" t="str" xml:space="preserve">
         <v xml:space="preserve"> 
-	  In this study, it was aimed to design the QR code-supported educational material related to 10th grade biology lesson heredity. In the study carried out in three stages, design and development research was used from quantitative research methods. In the first stage, in order to determine the subject of the research, Biology Concept Difficulty Survey were applied to a total of 506 high school students and teacher candidates. This survey was applied to 398 high school students in 9-12th grades in Bursa, and 108 freshmen students in Balıkesir University, Necatibey Faculty of Education. As a result; heredity section of heredity and biodiversity unit of 10th class biology subjects were determined as research subject. In the second stage, In order to determine why heredity is difficult, the Heredity Difficulties Survey was applied to 418 high school students in 10th grade and 22 biology teachers working in secondary education. As a result; while the students stated that the subject was detailed, the teachers stated that the concepts related to heredity were mixed together. In order to overcome these difficulties; students suggested simplify the content of heritability; teachers also suggested that videos about heritability subject should be given in QR code in textbooks. At the same stage, in order to provide a general evaluation of the heredity subject described in the biology lesson book of the 10th grade biology teacher by the teachers, Textbook Survey was applied to 22 biology teachers. As a result, scientific content level was found to be above the student level and remain incapable visual materials. As a result of in the same survey, biology teachers suggested that more visual materials should be given in sufficient numbers and scientific content should be at a level of students. At the end of the stage, in order to eliminate the difficulty of learning in the subject of heritability in line with all evaluations, a QR code-supported educational material was designed for use in the textbook or give as an activity paper in the lesson.</v>
+	  Biodiversity means both the economic and cultural wealth of a country. However, as a result of unconscious behaviour, our environment and biodiversity are threatened. Considering that this threat is increasing day by day, it is very important for students to be aware and educated. Leaving a livable world for future generations will only be possible with conscious, sensitive and sensible individuals who have developed its environmental literacy. In this study, it is aimed to research the effect of project-based education on biodiversity on high school students' perception of biology lesson. This study was conducted with 40 students studying in a public high school in Reşadiye district, in city of Tokat. In this study, for the attitudes of biology lesson of 10th grade students, one group pre-test post-test experimental weak design was used. This curriculum program prepared about biological diversity has implemented using project based teaching method. these students were given project proposals on the factors that threaten the biological diversity in their environment. Each student has presented his / her
+ix
+project to other friends in the group, thus, biodiversity and the factors that threaten biodiversity were examined in depth. Biology course attitude scale, which developed by Tosun (2011), was used to collect data. The data obtained from the pre-test and post-test of the scale questions were evaluated with descriptive statistics as well as Wilcoxon Signed Rank Test. As a result of the study, it was found that there was a significant difference between the pre-test and post-test scores of students, in favour of post-test, towards attitudes biology (significance level 0.003 (Z) -2,974). It was found that there was a significant difference between the first and second exam scores of the students based on the academic achievement variable, too (significance level 0,000 (Z) -5,277). A significant difference was found between the pre-test and post-test scores of the students to biology class attitude, according to the gender variable (Significance Level for female students is 0,019 (Z) -2,336; for male students it is 0,064 (Z) -1,853). According to this study results; It was understood that project based education on biodiversity, which applied to students, positively affected to students' attitudes towards biology course and academic achievement of biology course.</v>
       </c>
     </row>
   </sheetData>

</xml_diff>